<commit_message>
updated for nov. 18
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC9C927-2093-49BD-80B3-0916819D6091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6864F947-1029-43DE-AA95-5CCEC7850605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2655" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
@@ -21,7 +21,8 @@
     <sheet name="Books" sheetId="3" r:id="rId6"/>
     <sheet name="Betting" sheetId="10" state="hidden" r:id="rId7"/>
     <sheet name="Golf" sheetId="8" r:id="rId8"/>
-    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId9"/>
+    <sheet name="Bowling" sheetId="11" r:id="rId9"/>
+    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="388">
   <si>
     <t>Movie</t>
   </si>
@@ -1170,6 +1171,42 @@
   </si>
   <si>
     <t>Trill Factor</t>
+  </si>
+  <si>
+    <t>was giving the puck away. Did not play well. Good competition as well. Our forwards were not good. Couldn’t get the puck out</t>
+  </si>
+  <si>
+    <t>Planet Bowl</t>
+  </si>
+  <si>
+    <t>Companions</t>
+  </si>
+  <si>
+    <t>Mom, Trevor</t>
+  </si>
+  <si>
+    <t>Average Score</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Spares</t>
+  </si>
+  <si>
+    <t>Strikes</t>
+  </si>
+  <si>
+    <t>Spilt</t>
+  </si>
+  <si>
+    <t>Spilt Conversion</t>
+  </si>
+  <si>
+    <t>Gutters</t>
+  </si>
+  <si>
+    <t>Ball avg mph (1st ball)</t>
   </si>
 </sst>
 </file>
@@ -2575,10 +2612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,6 +3389,383 @@
       <c r="B30" t="s">
         <v>223</v>
       </c>
+      <c r="C30">
+        <v>7.1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45615</v>
+      </c>
+      <c r="B31" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FA9E0-547F-4AE8-9E5A-C35071F3E8D9}">
+  <dimension ref="B2:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M2" t="s">
+        <v>195</v>
+      </c>
+      <c r="N2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>45513</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>83</v>
+      </c>
+      <c r="N3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>45520</v>
+      </c>
+      <c r="C4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4">
+        <v>6.8</v>
+      </c>
+      <c r="F4">
+        <v>6.5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H4" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>6.5</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>4.5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5">
+        <v>6.1</v>
+      </c>
+      <c r="F5">
+        <v>5.9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <v>6.5</v>
+      </c>
+      <c r="K5">
+        <v>5.5</v>
+      </c>
+      <c r="L5">
+        <v>5.5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>219</v>
+      </c>
+      <c r="N5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>45550</v>
+      </c>
+      <c r="C6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>5.9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>7.5</v>
+      </c>
+      <c r="K6">
+        <v>6.5</v>
+      </c>
+      <c r="L6">
+        <v>5.8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>219</v>
+      </c>
+      <c r="N6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>45551</v>
+      </c>
+      <c r="C7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D7" t="s">
+        <v>331</v>
+      </c>
+      <c r="E7">
+        <v>6.7</v>
+      </c>
+      <c r="F7">
+        <v>6.8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>244</v>
+      </c>
+      <c r="H7" t="s">
+        <v>245</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>7.4</v>
+      </c>
+      <c r="K7">
+        <v>7.4</v>
+      </c>
+      <c r="L7">
+        <v>7.4</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>45565</v>
+      </c>
+      <c r="C8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>270</v>
+      </c>
+      <c r="I8">
+        <v>60</v>
+      </c>
+      <c r="J8">
+        <v>7.2</v>
+      </c>
+      <c r="K8">
+        <v>7.3</v>
+      </c>
+      <c r="L8">
+        <v>7.3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>45571</v>
+      </c>
+      <c r="C9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>6.7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>274</v>
+      </c>
+      <c r="H9" t="s">
+        <v>245</v>
+      </c>
+      <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <v>7.8</v>
+      </c>
+      <c r="K9">
+        <v>7.5</v>
+      </c>
+      <c r="L9">
+        <v>6.7</v>
+      </c>
+      <c r="M9" t="s">
+        <v>219</v>
+      </c>
+      <c r="N9" t="s">
+        <v>273</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3363,7 +3777,7 @@
   <dimension ref="B2:H42"/>
   <sheetViews>
     <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4311,7 +4725,7 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:H13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5042,7 +5456,7 @@
   <dimension ref="C4:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5620,7 +6034,7 @@
   <dimension ref="C3:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5859,341 +6273,86 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FA9E0-547F-4AE8-9E5A-C35071F3E8D9}">
-  <dimension ref="B2:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57673986-CD9F-49DA-9751-AFB1D94964E0}">
+  <dimension ref="B2:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>380</v>
       </c>
       <c r="E2" t="s">
-        <v>186</v>
+        <v>381</v>
       </c>
       <c r="F2" t="s">
-        <v>187</v>
+        <v>382</v>
       </c>
       <c r="G2" t="s">
-        <v>188</v>
+        <v>383</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>384</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>385</v>
       </c>
       <c r="J2" t="s">
-        <v>192</v>
+        <v>386</v>
       </c>
       <c r="K2" t="s">
-        <v>193</v>
+        <v>387</v>
       </c>
       <c r="L2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M2" t="s">
-        <v>195</v>
-      </c>
-      <c r="N2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>45613</v>
+      </c>
+      <c r="C3" t="s">
+        <v>377</v>
+      </c>
+      <c r="D3">
+        <v>127.3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>45513</v>
-      </c>
-      <c r="C3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H3" t="s">
-        <v>190</v>
-      </c>
       <c r="I3">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-      <c r="M3" t="s">
-        <v>83</v>
-      </c>
-      <c r="N3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>45520</v>
-      </c>
-      <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4">
-        <v>6.8</v>
-      </c>
-      <c r="F4">
-        <v>6.5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>199</v>
-      </c>
-      <c r="H4" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4">
-        <v>25</v>
-      </c>
-      <c r="J4">
-        <v>6.5</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
-        <v>4.5</v>
-      </c>
-      <c r="M4" t="s">
-        <v>83</v>
-      </c>
-      <c r="N4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5">
-        <v>6.1</v>
-      </c>
-      <c r="F5">
-        <v>5.9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H5" t="s">
-        <v>220</v>
-      </c>
-      <c r="I5">
-        <v>80</v>
-      </c>
-      <c r="J5">
-        <v>6.5</v>
-      </c>
-      <c r="K5">
-        <v>5.5</v>
-      </c>
-      <c r="L5">
-        <v>5.5</v>
-      </c>
-      <c r="M5" t="s">
-        <v>219</v>
-      </c>
-      <c r="N5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>45550</v>
-      </c>
-      <c r="C6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D6" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>5.9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H6" t="s">
-        <v>240</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>7.5</v>
-      </c>
-      <c r="K6">
-        <v>6.5</v>
-      </c>
-      <c r="L6">
-        <v>5.8</v>
-      </c>
-      <c r="M6" t="s">
-        <v>219</v>
-      </c>
-      <c r="N6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
-        <v>45551</v>
-      </c>
-      <c r="C7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D7" t="s">
-        <v>331</v>
-      </c>
-      <c r="E7">
-        <v>6.7</v>
-      </c>
-      <c r="F7">
-        <v>6.8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>244</v>
-      </c>
-      <c r="H7" t="s">
-        <v>245</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
-      <c r="J7">
-        <v>7.4</v>
-      </c>
-      <c r="K7">
-        <v>7.4</v>
-      </c>
-      <c r="L7">
-        <v>7.4</v>
-      </c>
-      <c r="M7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>45565</v>
-      </c>
-      <c r="C8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D8" t="s">
-        <v>331</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>270</v>
-      </c>
-      <c r="I8">
-        <v>60</v>
-      </c>
-      <c r="J8">
         <v>7.2</v>
       </c>
-      <c r="K8">
-        <v>7.3</v>
-      </c>
-      <c r="L8">
-        <v>7.3</v>
-      </c>
-      <c r="M8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
-        <v>45571</v>
-      </c>
-      <c r="C9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <v>6.7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>274</v>
-      </c>
-      <c r="H9" t="s">
-        <v>245</v>
-      </c>
-      <c r="I9">
-        <v>35</v>
-      </c>
-      <c r="J9">
-        <v>7.8</v>
-      </c>
-      <c r="K9">
-        <v>7.5</v>
-      </c>
-      <c r="L9">
-        <v>6.7</v>
-      </c>
-      <c r="M9" t="s">
-        <v>219</v>
-      </c>
-      <c r="N9" t="s">
-        <v>273</v>
+      <c r="L3" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for Nov 20.
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6864F947-1029-43DE-AA95-5CCEC7850605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B768E612-F01C-4706-BBCE-9EB348FB0F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="2670" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Betting" sheetId="10" state="hidden" r:id="rId7"/>
     <sheet name="Golf" sheetId="8" r:id="rId8"/>
     <sheet name="Bowling" sheetId="11" r:id="rId9"/>
-    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId10"/>
+    <sheet name="Job Aps" sheetId="12" r:id="rId10"/>
+    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="420">
   <si>
     <t>Movie</t>
   </si>
@@ -1207,6 +1208,102 @@
   </si>
   <si>
     <t>Ball avg mph (1st ball)</t>
+  </si>
+  <si>
+    <t>Analyst, Cancer Screening Analytics</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Ontario Health</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>November 23, 2024 (4 days left to apply)</t>
+  </si>
+  <si>
+    <t>Other Info</t>
+  </si>
+  <si>
+    <t>R107915</t>
+  </si>
+  <si>
+    <t>https://oh.wd3.myworkdayjobs.com/en-US/OH/job/Toronto-ON/Analyst--Health-Data-II_R107955</t>
+  </si>
+  <si>
+    <t>Analyst, Health Data</t>
+  </si>
+  <si>
+    <t>November 26, 2024 (7 days left to apply)</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/?vjk=dd81739d3c279da3</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>Atlantis IT group</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>Financial Planning Analyst - job post</t>
+  </si>
+  <si>
+    <t>Spectrum Health Care</t>
+  </si>
+  <si>
+    <t>Direct Website</t>
+  </si>
+  <si>
+    <t>Indeed</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/jobs?q=data&amp;l=Toronto%2C+ON&amp;vjk=14389fc4c61f4bb2</t>
+  </si>
+  <si>
+    <t>Economist / Research Analyst</t>
+  </si>
+  <si>
+    <t>UFCW Canada</t>
+  </si>
+  <si>
+    <t>played well. Good defense and passes. Decent shot</t>
+  </si>
+  <si>
+    <t>Burger Legend Etobicoke</t>
+  </si>
+  <si>
+    <t>8 30pm</t>
+  </si>
+  <si>
+    <t>Surpringly good - impressive. Gravy, everything, good</t>
+  </si>
+  <si>
+    <t>offense not the best</t>
+  </si>
+  <si>
+    <t>fell a couple times</t>
+  </si>
+  <si>
+    <t>passing was really good. Maybe passed 90% conversion. Won against a bunch of old guys</t>
+  </si>
+  <si>
+    <t>Technofeudalism</t>
   </si>
 </sst>
 </file>
@@ -2614,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,10 +3515,61 @@
       <c r="B31" t="s">
         <v>223</v>
       </c>
+      <c r="C31">
+        <v>7.9</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
+        <v>412</v>
+      </c>
+      <c r="J31" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45616</v>
+      </c>
+      <c r="B32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32">
+        <v>8.4</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>3</v>
+      </c>
+      <c r="I32" t="s">
+        <v>418</v>
+      </c>
+      <c r="J32" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3430,6 +3578,156 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
+  <dimension ref="B3:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" t="s">
+        <v>394</v>
+      </c>
+      <c r="F3" t="s">
+        <v>396</v>
+      </c>
+      <c r="G3" t="s">
+        <v>402</v>
+      </c>
+      <c r="I3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>43423</v>
+      </c>
+      <c r="C4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F4" t="s">
+        <v>397</v>
+      </c>
+      <c r="H4" t="s">
+        <v>407</v>
+      </c>
+      <c r="I4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>43423</v>
+      </c>
+      <c r="C5" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" t="s">
+        <v>393</v>
+      </c>
+      <c r="E5" t="s">
+        <v>400</v>
+      </c>
+      <c r="H5" t="s">
+        <v>407</v>
+      </c>
+      <c r="I5" t="s">
+        <v>398</v>
+      </c>
+      <c r="J5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>43424</v>
+      </c>
+      <c r="C6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6" t="s">
+        <v>403</v>
+      </c>
+      <c r="H6" t="s">
+        <v>408</v>
+      </c>
+      <c r="I6" t="s">
+        <v>401</v>
+      </c>
+      <c r="J6" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>43424</v>
+      </c>
+      <c r="C7" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" t="s">
+        <v>406</v>
+      </c>
+      <c r="H7" t="s">
+        <v>408</v>
+      </c>
+      <c r="I7" t="s">
+        <v>409</v>
+      </c>
+      <c r="J7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>43424</v>
+      </c>
+      <c r="C8" t="s">
+        <v>410</v>
+      </c>
+      <c r="D8" t="s">
+        <v>411</v>
+      </c>
+      <c r="H8" t="s">
+        <v>408</v>
+      </c>
+      <c r="I8" t="s">
+        <v>409</v>
+      </c>
+      <c r="J8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FA9E0-547F-4AE8-9E5A-C35071F3E8D9}">
   <dimension ref="B2:N9"/>
   <sheetViews>
@@ -5019,10 +5317,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="B4:I19"/>
+  <dimension ref="B4:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,6 +5742,32 @@
       </c>
       <c r="I19" t="s">
         <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>45616</v>
+      </c>
+      <c r="C20" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20">
+        <v>8.9</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>414</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -5681,8 +6005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5FEEB-3209-4CB9-ACB3-A3762D73B81E}">
   <dimension ref="C5:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5814,6 +6138,11 @@
       </c>
       <c r="I10" t="s">
         <v>305</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -6034,7 +6363,7 @@
   <dimension ref="C3:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated for week of dec 2
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B768E612-F01C-4706-BBCE-9EB348FB0F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7621B983-5CF6-47D6-8292-57E24D831DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="2505" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="1875" yWindow="210" windowWidth="28770" windowHeight="15570" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="476">
   <si>
     <t>Movie</t>
   </si>
@@ -1297,13 +1297,181 @@
     <t>offense not the best</t>
   </si>
   <si>
-    <t>fell a couple times</t>
-  </si>
-  <si>
     <t>passing was really good. Maybe passed 90% conversion. Won against a bunch of old guys</t>
   </si>
   <si>
     <t>Technofeudalism</t>
+  </si>
+  <si>
+    <t>fell a couple times. Sharped skates too much with the sharp rock</t>
+  </si>
+  <si>
+    <t>RESEARCH ANALYST 1</t>
+  </si>
+  <si>
+    <t>City of Toronto</t>
+  </si>
+  <si>
+    <t>Rabba Fine Foods</t>
+  </si>
+  <si>
+    <t>Financial Analyst</t>
+  </si>
+  <si>
+    <t>Financial Planning &amp; Operations Analyst</t>
+  </si>
+  <si>
+    <t>Zenduit Inc</t>
+  </si>
+  <si>
+    <t>https://ca.indeed.com/?vjk=ce0a6d5920421534</t>
+  </si>
+  <si>
+    <t>https://boomi.com/boomi-jobs/?gh_jid=5381151004&amp;gh_src=047aa44c4us</t>
+  </si>
+  <si>
+    <t>Business Intelligence Analyst</t>
+  </si>
+  <si>
+    <t>boomi</t>
+  </si>
+  <si>
+    <t>Data Visualization and Reporting Specialist</t>
+  </si>
+  <si>
+    <t>The Crump Group Inc.</t>
+  </si>
+  <si>
+    <t>Lioness</t>
+  </si>
+  <si>
+    <t>Bill Maher: Real Time</t>
+  </si>
+  <si>
+    <t>too many shots wide. I think the goalies scare me and I shoot too high</t>
+  </si>
+  <si>
+    <t>shot and skating was good</t>
+  </si>
+  <si>
+    <t>our team was stacked. I played ok played forward. Played with 4 girls on the other team was cool</t>
+  </si>
+  <si>
+    <t>Disapointing. New cop woman is interesting but can't save the plot</t>
+  </si>
+  <si>
+    <t>Paramount</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Discovery</t>
+  </si>
+  <si>
+    <t>Disney</t>
+  </si>
+  <si>
+    <t>HBO</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>https://u16314525.ct.sendgrid.net/ls/click?upn=u001.arcBAojtThf9ZVITG3zqo-2B9n3nSRh67FlnXvXD6XiqJzD7CYRwHkblu9roGGB8aJXoneV-2By6QkQmXvCDRYC3Ow-3D-3DYURQ_viv87QBHgf3cZPYRGDRhIf5Ije2xX6iaAQx9P2mzXowwskAoPVVtw45JYM7FIvj8JBUA6fmZnC9NmVTrLulWtVMD-2FWr-2F7XVC8phWzOOKkZ9qlpxOCEUPara8dwPEtlufvt4WLgRxGI35qKXKtA5T8H9YCBVtvWElldCp8-2FCevr4VOiuZSBalYYKquYMyi0AFjalBv3D7Bp48pM4KUOzB0A-3D-3D</t>
+  </si>
+  <si>
+    <t>Job Website</t>
+  </si>
+  <si>
+    <t>Phillip Morris</t>
+  </si>
+  <si>
+    <t>Ministry of Labour, Immigration, Training and Skills Development (Division: Strategic Policy Division / Data Analytics and Research Branch)</t>
+  </si>
+  <si>
+    <t>Job ID: 221695</t>
+  </si>
+  <si>
+    <t>Finished choosing by mid Jan then interviews then technical study</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>NRG PERSONNEL - Montréal, QC H1E 6M3</t>
+  </si>
+  <si>
+    <t>AppLovin - Toronto, ON</t>
+  </si>
+  <si>
+    <t>SUZUKI CANADA INC - Barrie, ON L4N 9Y2</t>
+  </si>
+  <si>
+    <t>Anora</t>
+  </si>
+  <si>
+    <t>Dark Comedy/Horror/Drama</t>
+  </si>
+  <si>
+    <t>Play Nice</t>
+  </si>
+  <si>
+    <t>defence and passing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offense </t>
+  </si>
+  <si>
+    <t>was paired with patey, we have no chem. He looks me off all the time. Not fun</t>
+  </si>
+  <si>
+    <t>9pm</t>
+  </si>
+  <si>
+    <t>boneless chicken buffalo</t>
+  </si>
+  <si>
+    <t>not good, would not recommend. Too saucy/vinegary</t>
+  </si>
+  <si>
+    <t>saw by myself at 12:45 on a Thursday. Love it. Old couple in front of me , long sex scene at the end left me unfortuable but funny nonetheless. I thought the movie was GREAT. The hencemen were top tier</t>
+  </si>
+  <si>
+    <t>It's Whats Inside</t>
+  </si>
+  <si>
+    <t>Horror?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">was ok, cool idea. Recommended from a friend. Not into body shifting. Filming was artsy and fun </t>
+  </si>
+  <si>
+    <t>The Old Man</t>
+  </si>
+  <si>
+    <t>X Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shooting wide. </t>
+  </si>
+  <si>
+    <t>Can shoot harder and aim better. Setup some good plays. Won close game</t>
+  </si>
+  <si>
+    <t>Outdoor Rink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passing </t>
+  </si>
+  <si>
+    <t>fun time in the sun. at 12 30 could hardly see in the sun! had a big fall I hit greg and speared him. Oops! I was ok. Hit boards hard and phone went flying</t>
+  </si>
+  <si>
+    <t>puck handling?</t>
   </si>
 </sst>
 </file>
@@ -2709,10 +2877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3554,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -3566,10 +3734,155 @@
         <v>3</v>
       </c>
       <c r="I32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J32" t="s">
-        <v>417</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>45618</v>
+      </c>
+      <c r="B33" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33">
+        <v>7.9</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33" t="s">
+        <v>435</v>
+      </c>
+      <c r="J33" t="s">
+        <v>434</v>
+      </c>
+      <c r="K33" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45623</v>
+      </c>
+      <c r="B34" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34">
+        <v>7.5</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>458</v>
+      </c>
+      <c r="J34" t="s">
+        <v>459</v>
+      </c>
+      <c r="K34" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>45627</v>
+      </c>
+      <c r="B35" t="s">
+        <v>472</v>
+      </c>
+      <c r="C35">
+        <v>7.8</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>473</v>
+      </c>
+      <c r="J35" t="s">
+        <v>475</v>
+      </c>
+      <c r="K35" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>45628</v>
+      </c>
+      <c r="B36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36">
+        <v>8.1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>458</v>
+      </c>
+      <c r="J36" t="s">
+        <v>470</v>
+      </c>
+      <c r="K36" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45630</v>
       </c>
     </row>
   </sheetData>
@@ -3579,10 +3892,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="B3:J8"/>
+  <dimension ref="B3:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3720,6 +4033,167 @@
       </c>
       <c r="J8" t="s">
         <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>43425</v>
+      </c>
+      <c r="C9" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" t="s">
+        <v>421</v>
+      </c>
+      <c r="H9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>43425</v>
+      </c>
+      <c r="C10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H10" t="s">
+        <v>408</v>
+      </c>
+      <c r="I10" t="s">
+        <v>426</v>
+      </c>
+      <c r="J10" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>43425</v>
+      </c>
+      <c r="C11" t="s">
+        <v>424</v>
+      </c>
+      <c r="D11" t="s">
+        <v>425</v>
+      </c>
+      <c r="H11" t="s">
+        <v>408</v>
+      </c>
+      <c r="I11" t="s">
+        <v>426</v>
+      </c>
+      <c r="J11" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>43425</v>
+      </c>
+      <c r="C12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D12" t="s">
+        <v>429</v>
+      </c>
+      <c r="H12" t="s">
+        <v>407</v>
+      </c>
+      <c r="I12" t="s">
+        <v>427</v>
+      </c>
+      <c r="J12" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>43425</v>
+      </c>
+      <c r="C13" t="s">
+        <v>430</v>
+      </c>
+      <c r="D13" t="s">
+        <v>431</v>
+      </c>
+      <c r="H13" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>43431</v>
+      </c>
+      <c r="C14" t="s">
+        <v>450</v>
+      </c>
+      <c r="D14" t="s">
+        <v>447</v>
+      </c>
+      <c r="F14" t="s">
+        <v>448</v>
+      </c>
+      <c r="G14" t="s">
+        <v>449</v>
+      </c>
+      <c r="H14" t="s">
+        <v>445</v>
+      </c>
+      <c r="I14" t="s">
+        <v>444</v>
+      </c>
+      <c r="J14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <v>43431</v>
+      </c>
+      <c r="D15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>43431</v>
+      </c>
+      <c r="C16" t="s">
+        <v>451</v>
+      </c>
+      <c r="D16" t="s">
+        <v>452</v>
+      </c>
+      <c r="H16" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>43431</v>
+      </c>
+      <c r="C17" t="s">
+        <v>451</v>
+      </c>
+      <c r="D17" t="s">
+        <v>453</v>
+      </c>
+      <c r="H17" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>43431</v>
+      </c>
+      <c r="C18" t="s">
+        <v>404</v>
+      </c>
+      <c r="D18" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4072,10 +4546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="B2:H42"/>
+  <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5013,6 +5487,52 @@
         <v>374</v>
       </c>
     </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>45624</v>
+      </c>
+      <c r="C43" t="s">
+        <v>455</v>
+      </c>
+      <c r="D43">
+        <v>9.4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>456</v>
+      </c>
+      <c r="F43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" t="s">
+        <v>87</v>
+      </c>
+      <c r="H43" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>45638</v>
+      </c>
+      <c r="C44" t="s">
+        <v>465</v>
+      </c>
+      <c r="D44">
+        <v>6.6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>466</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" t="s">
+        <v>467</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5020,10 +5540,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="B2:H13"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5031,10 +5551,10 @@
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -5051,13 +5571,16 @@
         <v>39</v>
       </c>
       <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>45475</v>
       </c>
@@ -5074,13 +5597,16 @@
         <v>49</v>
       </c>
       <c r="G3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H3" t="s">
         <v>100</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>45489</v>
       </c>
@@ -5097,13 +5623,16 @@
         <v>83</v>
       </c>
       <c r="G4" t="s">
+        <v>443</v>
+      </c>
+      <c r="H4" t="s">
         <v>143</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>45519</v>
       </c>
@@ -5120,13 +5649,16 @@
         <v>49</v>
       </c>
       <c r="G5" t="s">
+        <v>441</v>
+      </c>
+      <c r="H5" t="s">
         <v>177</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>45515</v>
       </c>
@@ -5143,13 +5675,16 @@
         <v>49</v>
       </c>
       <c r="G6" t="s">
+        <v>442</v>
+      </c>
+      <c r="H6" t="s">
         <v>180</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>45541</v>
       </c>
@@ -5166,13 +5701,16 @@
         <v>49</v>
       </c>
       <c r="G7" t="s">
+        <v>443</v>
+      </c>
+      <c r="H7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>45547</v>
       </c>
@@ -5189,13 +5727,16 @@
         <v>49</v>
       </c>
       <c r="G8" t="s">
+        <v>443</v>
+      </c>
+      <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>45560</v>
       </c>
@@ -5212,13 +5753,16 @@
         <v>49</v>
       </c>
       <c r="G9" t="s">
+        <v>440</v>
+      </c>
+      <c r="H9" t="s">
         <v>284</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>45598</v>
       </c>
@@ -5235,13 +5779,16 @@
         <v>49</v>
       </c>
       <c r="G10" t="s">
+        <v>439</v>
+      </c>
+      <c r="H10" t="s">
         <v>325</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>45600</v>
       </c>
@@ -5258,13 +5805,16 @@
         <v>49</v>
       </c>
       <c r="G11" t="s">
+        <v>440</v>
+      </c>
+      <c r="H11" t="s">
         <v>325</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>45604</v>
       </c>
@@ -5281,13 +5831,16 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
+        <v>440</v>
+      </c>
+      <c r="H12" t="s">
         <v>325</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>45610</v>
       </c>
@@ -5304,10 +5857,89 @@
         <v>49</v>
       </c>
       <c r="G13" t="s">
+        <v>438</v>
+      </c>
+      <c r="H13" t="s">
         <v>253</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>366</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>45624</v>
+      </c>
+      <c r="C14" t="s">
+        <v>365</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>6.4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
+        <v>438</v>
+      </c>
+      <c r="H14" t="s">
+        <v>253</v>
+      </c>
+      <c r="I14" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>432</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>45620</v>
+      </c>
+      <c r="C16" t="s">
+        <v>433</v>
+      </c>
+      <c r="E16">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>468</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>469</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5317,10 +5949,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="B4:I20"/>
+  <dimension ref="B4:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5770,6 +6402,32 @@
         <v>415</v>
       </c>
     </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>45624</v>
+      </c>
+      <c r="C21" t="s">
+        <v>413</v>
+      </c>
+      <c r="D21">
+        <v>7.1</v>
+      </c>
+      <c r="E21">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" t="s">
+        <v>461</v>
+      </c>
+      <c r="H21" t="s">
+        <v>462</v>
+      </c>
+      <c r="I21" t="s">
+        <v>463</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5780,7 +6438,7 @@
   <dimension ref="C4:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6005,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5FEEB-3209-4CB9-ACB3-A3762D73B81E}">
   <dimension ref="C5:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6142,7 +6800,12 @@
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>419</v>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
@@ -6363,7 +7026,7 @@
   <dimension ref="C3:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated for dec 10
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7621B983-5CF6-47D6-8292-57E24D831DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC918918-0046-43B8-86D5-FB82D7FC4B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="210" windowWidth="28770" windowHeight="15570" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15570" activeTab="9" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Golf" sheetId="8" r:id="rId8"/>
     <sheet name="Bowling" sheetId="11" r:id="rId9"/>
     <sheet name="Job Aps" sheetId="12" r:id="rId10"/>
-    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId11"/>
+    <sheet name="Tacos" sheetId="13" r:id="rId11"/>
+    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="498">
   <si>
     <t>Movie</t>
   </si>
@@ -1462,9 +1463,6 @@
     <t>Can shoot harder and aim better. Setup some good plays. Won close game</t>
   </si>
   <si>
-    <t>Outdoor Rink</t>
-  </si>
-  <si>
     <t xml:space="preserve">passing </t>
   </si>
   <si>
@@ -1472,6 +1470,75 @@
   </si>
   <si>
     <t>puck handling?</t>
+  </si>
+  <si>
+    <t>Penalty Minutes</t>
+  </si>
+  <si>
+    <t>Penalty Type</t>
+  </si>
+  <si>
+    <t>Tripping</t>
+  </si>
+  <si>
+    <t>good game. Kicked their ass. They were not very good. 3 man d</t>
+  </si>
+  <si>
+    <t>shooting could be harder slap it higher</t>
+  </si>
+  <si>
+    <t>Rogue Heroes</t>
+  </si>
+  <si>
+    <t>Action, History</t>
+  </si>
+  <si>
+    <t>Conclave</t>
+  </si>
+  <si>
+    <t>Juror 2</t>
+  </si>
+  <si>
+    <t>great. Disliked the climax and ending</t>
+  </si>
+  <si>
+    <t>love a good juror movie. Clint eastwood is a master of cinema</t>
+  </si>
+  <si>
+    <t>Project Bluegroup</t>
+  </si>
+  <si>
+    <t>Drama, History</t>
+  </si>
+  <si>
+    <t>Enjoyed it</t>
+  </si>
+  <si>
+    <t>Westmall Outdoor Rink</t>
+  </si>
+  <si>
+    <t>stick handling and shot</t>
+  </si>
+  <si>
+    <t>work on stick handling more</t>
+  </si>
+  <si>
+    <t>good snack after some outdoor hockey with my friend Conor</t>
+  </si>
+  <si>
+    <t>Tahini</t>
+  </si>
+  <si>
+    <t>3pm</t>
+  </si>
+  <si>
+    <t>surprisingly not bad. Fallfael I got wasn't that good. Probably not going back</t>
+  </si>
+  <si>
+    <t>First Round</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -2877,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,7 +2956,7 @@
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2916,16 +2983,22 @@
         <v>329</v>
       </c>
       <c r="I1" t="s">
+        <v>475</v>
+      </c>
+      <c r="J1" t="s">
+        <v>476</v>
+      </c>
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45454</v>
       </c>
@@ -2941,17 +3014,17 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>44</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>45</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45468</v>
       </c>
@@ -2967,17 +3040,17 @@
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>76</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>77</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45475</v>
       </c>
@@ -2993,17 +3066,17 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>105</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>103</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45482</v>
       </c>
@@ -3019,17 +3092,17 @@
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>112</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>111</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45489</v>
       </c>
@@ -3045,17 +3118,17 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>124</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45496</v>
       </c>
@@ -3071,17 +3144,17 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>154</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45503</v>
       </c>
@@ -3097,14 +3170,14 @@
       <c r="E8">
         <v>2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>44</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45504</v>
       </c>
@@ -3120,17 +3193,17 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>157</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>159</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45510</v>
       </c>
@@ -3146,14 +3219,14 @@
       <c r="E10">
         <v>3</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>171</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45518</v>
       </c>
@@ -3169,17 +3242,17 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>171</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45524</v>
       </c>
@@ -3195,14 +3268,14 @@
       <c r="E12">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>201</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45543</v>
       </c>
@@ -3218,17 +3291,17 @@
       <c r="E13">
         <v>3</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>44</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>103</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45552</v>
       </c>
@@ -3244,17 +3317,17 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>236</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>234</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45555</v>
       </c>
@@ -3270,17 +3343,17 @@
       <c r="E15">
         <v>2</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>250</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>249</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45553</v>
       </c>
@@ -3296,17 +3369,17 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>251</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>246</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45562</v>
       </c>
@@ -3322,17 +3395,17 @@
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>258</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>259</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45567</v>
       </c>
@@ -3351,11 +3424,11 @@
       <c r="G18">
         <v>2</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45569</v>
       </c>
@@ -3371,11 +3444,11 @@
       <c r="E19">
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45574</v>
       </c>
@@ -3394,11 +3467,11 @@
       <c r="G20">
         <v>2</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45576</v>
       </c>
@@ -3417,11 +3490,11 @@
       <c r="F21">
         <v>4</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45581</v>
       </c>
@@ -3443,11 +3516,11 @@
       <c r="G22">
         <v>1</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45583</v>
       </c>
@@ -3469,11 +3542,11 @@
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45590</v>
       </c>
@@ -3498,11 +3571,11 @@
       <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45595</v>
       </c>
@@ -3527,11 +3600,11 @@
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45597</v>
       </c>
@@ -3556,11 +3629,11 @@
       <c r="H26">
         <v>3</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45600</v>
       </c>
@@ -3585,11 +3658,11 @@
       <c r="H27">
         <v>5</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45604</v>
       </c>
@@ -3614,11 +3687,11 @@
       <c r="H28">
         <v>4</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45609</v>
       </c>
@@ -3643,11 +3716,11 @@
       <c r="H29">
         <v>3</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45611</v>
       </c>
@@ -3672,11 +3745,11 @@
       <c r="H30">
         <v>2</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45615</v>
       </c>
@@ -3701,14 +3774,14 @@
       <c r="H31">
         <v>3</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>412</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45616</v>
       </c>
@@ -3733,14 +3806,14 @@
       <c r="H32">
         <v>3</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>417</v>
       </c>
-      <c r="J32" t="s">
+      <c r="L32" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45618</v>
       </c>
@@ -3765,17 +3838,17 @@
       <c r="H33">
         <v>4</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>435</v>
       </c>
-      <c r="J33" t="s">
+      <c r="L33" t="s">
         <v>434</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45623</v>
       </c>
@@ -3800,22 +3873,22 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>458</v>
       </c>
-      <c r="J34" t="s">
+      <c r="L34" t="s">
         <v>459</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45627</v>
       </c>
       <c r="B35" t="s">
-        <v>472</v>
+        <v>489</v>
       </c>
       <c r="C35">
         <v>7.8</v>
@@ -3835,17 +3908,17 @@
       <c r="H35">
         <v>4</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
+        <v>472</v>
+      </c>
+      <c r="L35" t="s">
+        <v>474</v>
+      </c>
+      <c r="M35" t="s">
         <v>473</v>
       </c>
-      <c r="J35" t="s">
-        <v>475</v>
-      </c>
-      <c r="K35" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45628</v>
       </c>
@@ -3870,19 +3943,113 @@
       <c r="H36">
         <v>4</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>458</v>
       </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
         <v>470</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45630</v>
+      </c>
+      <c r="B37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>477</v>
+      </c>
+      <c r="K37" t="s">
+        <v>458</v>
+      </c>
+      <c r="L37" t="s">
+        <v>479</v>
+      </c>
+      <c r="M37" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45634</v>
+      </c>
+      <c r="B38" t="s">
+        <v>489</v>
+      </c>
+      <c r="C38">
+        <v>7.8</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45635</v>
+      </c>
+      <c r="B39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39">
+        <v>7.9</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="K39" t="s">
+        <v>458</v>
+      </c>
+      <c r="L39" t="s">
+        <v>490</v>
+      </c>
+      <c r="M39" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -3892,10 +4059,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="B3:J18"/>
+  <dimension ref="B3:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3903,7 +4070,7 @@
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3925,8 +4092,11 @@
       <c r="I3" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>43423</v>
       </c>
@@ -3951,8 +4121,11 @@
       <c r="J4" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>43423</v>
       </c>
@@ -3975,7 +4148,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>43424</v>
       </c>
@@ -3995,7 +4168,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>43424</v>
       </c>
@@ -4015,7 +4188,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>43424</v>
       </c>
@@ -4035,7 +4208,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>43425</v>
       </c>
@@ -4049,7 +4222,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>43425</v>
       </c>
@@ -4069,7 +4242,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>43425</v>
       </c>
@@ -4089,7 +4262,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>43425</v>
       </c>
@@ -4109,7 +4282,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>43425</v>
       </c>
@@ -4123,7 +4296,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>43431</v>
       </c>
@@ -4149,7 +4322,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>43431</v>
       </c>
@@ -4157,7 +4330,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>43431</v>
       </c>
@@ -4202,6 +4375,47 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD007E7E-FC98-4AF1-99C6-188F4344C8E3}">
+  <dimension ref="B4:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FA9E0-547F-4AE8-9E5A-C35071F3E8D9}">
   <dimension ref="B2:N9"/>
   <sheetViews>
@@ -4546,10 +4760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="B2:H44"/>
+  <dimension ref="B1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4559,165 +4773,188 @@
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>45437</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>9.1999999999999993</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
-        <v>45437</v>
+        <v>45439</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>9.1999999999999993</v>
+        <v>8.6</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>49</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
-        <v>45439</v>
+        <v>45441</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D4">
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
         <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>45441</v>
+      <c r="B5" s="2">
+        <v>45448</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>8.8000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="E5" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
         <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>45448</v>
+        <v>45453</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>6.1</v>
+        <v>7.4</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
         <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>45453</v>
+        <v>45454</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D7">
-        <v>7.4</v>
+        <v>5.3</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
         <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>45454</v>
+        <v>45455</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D8">
-        <v>5.3</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -4725,79 +4962,79 @@
         <v>45455</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D9">
-        <v>9.1999999999999993</v>
+        <v>5.4</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
         <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>45455</v>
+        <v>45473</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D10">
-        <v>5.4</v>
+        <v>7.9</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="F10" t="s">
         <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>45473</v>
+        <v>45476</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11">
-        <v>7.9</v>
+        <v>107</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>45476</v>
+        <v>45483</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="5">
-        <v>8</v>
+        <v>108</v>
+      </c>
+      <c r="D12">
+        <v>6.4</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -4806,21 +5043,21 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>45483</v>
+        <v>45484</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D13">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -4829,47 +5066,47 @@
         <v>49</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>45484</v>
+        <v>45486</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="D14">
-        <v>6.1</v>
+        <v>7.5</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>45486</v>
+        <v>45489</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="D15">
-        <v>7.5</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="F15" t="s">
         <v>49</v>
@@ -4878,41 +5115,41 @@
         <v>89</v>
       </c>
       <c r="H15" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>45489</v>
+        <v>45490</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D16">
-        <v>9.1999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
         <v>49</v>
       </c>
       <c r="G16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H16" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>45490</v>
+        <v>45493</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="D17">
-        <v>8.3000000000000007</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -4921,24 +5158,24 @@
         <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>45493</v>
+        <v>45497</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D18">
-        <v>9.3000000000000007</v>
+        <v>9.1</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
         <v>49</v>
@@ -4947,41 +5184,41 @@
         <v>89</v>
       </c>
       <c r="H18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>45497</v>
+        <v>45507</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="D19">
-        <v>9.1</v>
+        <v>6.5</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>85</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H19" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>45507</v>
+        <v>45488</v>
       </c>
       <c r="C20" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D20">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
       <c r="E20" t="s">
         <v>85</v>
@@ -4993,7 +5230,7 @@
         <v>91</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -5001,13 +5238,13 @@
         <v>45488</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D21">
-        <v>6.4</v>
+        <v>5.9</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
         <v>83</v>
@@ -5016,18 +5253,18 @@
         <v>91</v>
       </c>
       <c r="H21" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>45488</v>
+        <v>45483</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D22">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="E22" t="s">
         <v>10</v>
@@ -5039,113 +5276,113 @@
         <v>91</v>
       </c>
       <c r="H22" t="s">
-        <v>21</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>45483</v>
+        <v>45521</v>
       </c>
       <c r="C23" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="D23">
-        <v>6.1</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>206</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G23" t="s">
-        <v>91</v>
+        <v>207</v>
       </c>
       <c r="H23" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>45521</v>
+        <v>45529</v>
       </c>
       <c r="C24" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D24">
-        <v>9.3000000000000007</v>
+        <v>6.4</v>
       </c>
       <c r="E24" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="F24" t="s">
         <v>49</v>
       </c>
       <c r="G24" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="H24" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>45529</v>
+        <v>45530</v>
       </c>
       <c r="C25" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D25">
-        <v>6.4</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="E25" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F25" t="s">
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>212</v>
+        <v>89</v>
       </c>
       <c r="H25" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>45530</v>
+        <v>45551</v>
       </c>
       <c r="C26" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="D26">
-        <v>8.6999999999999993</v>
+        <v>6.3</v>
       </c>
       <c r="E26" t="s">
-        <v>214</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
         <v>49</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>231</v>
       </c>
       <c r="H26" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>45551</v>
+        <v>45556</v>
       </c>
       <c r="C27" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="D27">
-        <v>6.3</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>253</v>
       </c>
       <c r="F27" t="s">
         <v>49</v>
@@ -5154,21 +5391,21 @@
         <v>231</v>
       </c>
       <c r="H27" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>45556</v>
+        <v>45559</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>6.2</v>
       </c>
       <c r="E28" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="F28" t="s">
         <v>49</v>
@@ -5177,21 +5414,21 @@
         <v>231</v>
       </c>
       <c r="H28" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>45559</v>
+        <v>45564</v>
       </c>
       <c r="C29" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D29">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
       <c r="E29" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="F29" t="s">
         <v>49</v>
@@ -5200,7 +5437,7 @@
         <v>231</v>
       </c>
       <c r="H29" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -5208,56 +5445,56 @@
         <v>45564</v>
       </c>
       <c r="C30" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D30">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>256</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G30" t="s">
         <v>231</v>
       </c>
       <c r="H30" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
-        <v>45564</v>
+        <v>45566</v>
       </c>
       <c r="C31" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>8.5</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G31" t="s">
         <v>231</v>
       </c>
       <c r="H31" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
-        <v>45566</v>
+        <v>45570</v>
       </c>
       <c r="C32" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D32">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -5266,21 +5503,21 @@
         <v>49</v>
       </c>
       <c r="G32" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
       <c r="H32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
-        <v>45570</v>
+        <v>45574</v>
       </c>
       <c r="C33" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D33">
-        <v>7.5</v>
+        <v>7.9</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -5292,7 +5529,7 @@
         <v>277</v>
       </c>
       <c r="H33" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -5300,10 +5537,10 @@
         <v>45574</v>
       </c>
       <c r="C34" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D34">
-        <v>7.9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -5315,18 +5552,18 @@
         <v>277</v>
       </c>
       <c r="H34" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
-        <v>45574</v>
+        <v>45575</v>
       </c>
       <c r="C35" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D35">
-        <v>8.3000000000000007</v>
+        <v>6.6</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -5338,53 +5575,53 @@
         <v>277</v>
       </c>
       <c r="H35" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
-        <v>45575</v>
+        <v>45578</v>
       </c>
       <c r="C36" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="D36">
-        <v>6.6</v>
+        <v>7.9</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F36" t="s">
         <v>49</v>
       </c>
       <c r="G36" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
       <c r="H36" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
-        <v>45578</v>
+        <v>45585</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D37">
-        <v>7.9</v>
+        <v>6.5</v>
       </c>
       <c r="E37" t="s">
-        <v>100</v>
+        <v>297</v>
       </c>
       <c r="F37" t="s">
         <v>49</v>
       </c>
       <c r="G37" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="H37" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -5392,13 +5629,13 @@
         <v>45585</v>
       </c>
       <c r="C38" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D38">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="E38" t="s">
-        <v>297</v>
+        <v>12</v>
       </c>
       <c r="F38" t="s">
         <v>49</v>
@@ -5407,130 +5644,153 @@
         <v>300</v>
       </c>
       <c r="H38" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="2">
-        <v>45585</v>
-      </c>
       <c r="C39" t="s">
-        <v>299</v>
-      </c>
-      <c r="D39">
-        <v>6.6</v>
-      </c>
-      <c r="E39" t="s">
+        <v>317</v>
+      </c>
+      <c r="G39" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>45584</v>
+      </c>
+      <c r="C40" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40">
+        <v>5.9</v>
+      </c>
+      <c r="E40" t="s">
         <v>12</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>49</v>
       </c>
-      <c r="G39" t="s">
-        <v>300</v>
-      </c>
-      <c r="H39" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>317</v>
-      </c>
       <c r="G40" t="s">
-        <v>318</v>
+        <v>231</v>
+      </c>
+      <c r="H40" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
-        <v>45584</v>
+        <v>45610</v>
       </c>
       <c r="C41" t="s">
-        <v>319</v>
+        <v>372</v>
       </c>
       <c r="D41">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>373</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G41" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="H41" t="s">
-        <v>320</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
-        <v>45610</v>
+        <v>45624</v>
       </c>
       <c r="C42" t="s">
-        <v>372</v>
+        <v>455</v>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>9.4</v>
       </c>
       <c r="E42" t="s">
-        <v>373</v>
+        <v>456</v>
       </c>
       <c r="F42" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="G42" t="s">
-        <v>300</v>
+        <v>87</v>
       </c>
       <c r="H42" t="s">
-        <v>374</v>
+        <v>464</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
-        <v>45624</v>
+        <v>45638</v>
       </c>
       <c r="C43" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="D43">
-        <v>9.4</v>
+        <v>6.6</v>
       </c>
       <c r="E43" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="F43" t="s">
         <v>49</v>
       </c>
       <c r="G43" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H43" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
-        <v>45638</v>
+        <v>45633</v>
       </c>
       <c r="C44" t="s">
-        <v>465</v>
+        <v>482</v>
       </c>
       <c r="D44">
-        <v>6.6</v>
+        <v>8.1</v>
       </c>
       <c r="E44" t="s">
-        <v>466</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
         <v>49</v>
       </c>
       <c r="G44" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
       <c r="H44" t="s">
-        <v>467</v>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>45635</v>
+      </c>
+      <c r="C45" t="s">
+        <v>483</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" t="s">
+        <v>231</v>
+      </c>
+      <c r="H45" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -5540,10 +5800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="B2:I18"/>
+  <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5926,7 +6186,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>468</v>
       </c>
@@ -5934,12 +6194,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>469</v>
       </c>
       <c r="D18">
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>480</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>212</v>
+      </c>
+      <c r="H19" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>486</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>8.1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" t="s">
+        <v>442</v>
+      </c>
+      <c r="H20" t="s">
+        <v>487</v>
+      </c>
+      <c r="I20" t="s">
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -5949,10 +6246,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="B4:I21"/>
+  <dimension ref="B4:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6428,6 +6725,58 @@
         <v>463</v>
       </c>
     </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
+        <v>45633</v>
+      </c>
+      <c r="C22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D22">
+        <v>7.8</v>
+      </c>
+      <c r="E22">
+        <v>8.85</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>81</v>
+      </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>45635</v>
+      </c>
+      <c r="C23" t="s">
+        <v>493</v>
+      </c>
+      <c r="D23">
+        <v>7.4</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>494</v>
+      </c>
+      <c r="H23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" t="s">
+        <v>495</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6438,7 +6787,7 @@
   <dimension ref="C4:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated for dec 22
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2855059E-7C51-4D90-A307-14E490EC4135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC88ECA-BF72-454F-AA2F-0CAD9C65087D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="526">
   <si>
     <t>Movie</t>
   </si>
@@ -1589,6 +1589,39 @@
   </si>
   <si>
     <t>Mexico Bowl</t>
+  </si>
+  <si>
+    <t>La Palma</t>
+  </si>
+  <si>
+    <t>Meh. Kind of boring</t>
+  </si>
+  <si>
+    <t>Ready or Not</t>
+  </si>
+  <si>
+    <t>good horror movie. And funny</t>
+  </si>
+  <si>
+    <t>I Spit on Your Grave</t>
+  </si>
+  <si>
+    <t>Top Gun Burger</t>
+  </si>
+  <si>
+    <t>watched with denisse. Wow she is amazing at watching horrors this one was absolutely tough to watch. There was 2 rape scenes and at one of the major revenge scenes he cut off this guy's pen1s with garden scissors and shoved it in his mouth haha!</t>
+  </si>
+  <si>
+    <t>Jason Schreier</t>
+  </si>
+  <si>
+    <t>The Snakehead</t>
+  </si>
+  <si>
+    <t>Patrick Radden Keefe</t>
+  </si>
+  <si>
+    <t>good book very interesting. Nice to hear the history of how everything rose and fall. Much lessons to be had</t>
   </si>
 </sst>
 </file>
@@ -2997,7 +3030,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4783,10 +4816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5946,6 +5979,52 @@
         <v>510</v>
       </c>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>45647</v>
+      </c>
+      <c r="B51" t="s">
+        <v>517</v>
+      </c>
+      <c r="C51">
+        <v>7.8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>214</v>
+      </c>
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>91</v>
+      </c>
+      <c r="G51" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>45648</v>
+      </c>
+      <c r="B52" t="s">
+        <v>519</v>
+      </c>
+      <c r="C52">
+        <v>6.1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>49</v>
+      </c>
+      <c r="F52" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52" t="s">
+        <v>521</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5953,10 +6032,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6398,6 +6477,32 @@
         <v>488</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>45647</v>
+      </c>
+      <c r="B20" t="s">
+        <v>515</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>6.4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>439</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" t="s">
+        <v>516</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6408,7 +6513,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6505,7 +6610,7 @@
         <v>67</v>
       </c>
       <c r="C4">
-        <v>8.9</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -6557,7 +6662,7 @@
         <v>79</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="D6">
         <v>9</v>
@@ -6661,7 +6766,7 @@
         <v>161</v>
       </c>
       <c r="C10">
-        <v>9.1</v>
+        <v>8.9</v>
       </c>
       <c r="D10">
         <v>10</v>
@@ -6713,7 +6818,7 @@
         <v>225</v>
       </c>
       <c r="C12">
-        <v>9.3000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D12">
         <v>15</v>
@@ -6760,6 +6865,9 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>45592</v>
+      </c>
+      <c r="B14" t="s">
+        <v>520</v>
       </c>
       <c r="C14">
         <v>5.6</v>
@@ -7169,10 +7277,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF5FEEB-3209-4CB9-ACB3-A3762D73B81E}">
-  <dimension ref="C5:I13"/>
+  <dimension ref="C5:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7312,8 +7420,26 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="3">
+        <v>45587</v>
+      </c>
       <c r="D12" t="s">
         <v>457</v>
+      </c>
+      <c r="E12" t="s">
+        <v>522</v>
+      </c>
+      <c r="F12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12">
+        <v>8.5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.3">
@@ -7327,6 +7453,20 @@
         <v>135</v>
       </c>
       <c r="G13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>523</v>
+      </c>
+      <c r="E14" t="s">
+        <v>524</v>
+      </c>
+      <c r="F14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" t="s">
         <v>83</v>
       </c>
     </row>
@@ -7534,7 +7674,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated for jan 5, 2025
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9A5A8F-71EA-45EA-B33D-DDF14CFEFBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFFA25F-47CA-4947-849F-EF266842997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1200" windowWidth="22155" windowHeight="11700" activeTab="2" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="1200" yWindow="1200" windowWidth="22155" windowHeight="11700" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Golf" sheetId="8" r:id="rId8"/>
     <sheet name="Bowling" sheetId="11" r:id="rId9"/>
     <sheet name="Job Aps" sheetId="12" r:id="rId10"/>
-    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId11"/>
+    <sheet name="Concerts" sheetId="13" r:id="rId11"/>
+    <sheet name="Dates" sheetId="9" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="556">
   <si>
     <t>Movie</t>
   </si>
@@ -1642,13 +1643,10 @@
     <t>good movie but I didn't like it. The female lead annoyed me. Dafoe was clearly the best</t>
   </si>
   <si>
-    <t>Financeit</t>
-  </si>
-  <si>
-    <t>Analyst, Risk Analystics &amp; Reporting</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4094726918</t>
+    <t>Business Intelligence Specialist</t>
+  </si>
+  <si>
+    <t>2iSolutions Inc.</t>
   </si>
   <si>
     <t>Linkedin</t>
@@ -1660,22 +1658,61 @@
     <t>Enwave</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/jobs/view/4102539461/</t>
-  </si>
-  <si>
-    <t>Research and Data Analyst</t>
-  </si>
-  <si>
-    <t>Ontario Securities Commission</t>
-  </si>
-  <si>
-    <t>Analyst, Strategy</t>
-  </si>
-  <si>
-    <t>Squid Game</t>
-  </si>
-  <si>
-    <t>Landman</t>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Accompanied</t>
+  </si>
+  <si>
+    <t>Speed and passing</t>
+  </si>
+  <si>
+    <t>tried longer stick think I have more power and reach. Keep using. Scored only goal and it was on AA goalie. Was great</t>
+  </si>
+  <si>
+    <t>Wind em up more for snap shots. You are too hesitate! You got a good pass and you should just clap it right in</t>
+  </si>
+  <si>
+    <t>Emerson's dad's band. Was surprisingly good. Played covers and some orgionals. Almost packed horshoe. 3 sets for $15</t>
+  </si>
+  <si>
+    <t>Conor, Seb</t>
+  </si>
+  <si>
+    <t>Horseshoe</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>good snack. Friend had to leave early from lunch, was hungry</t>
+  </si>
+  <si>
+    <t>Small Things Like These</t>
+  </si>
+  <si>
+    <t>Brutalist</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>solid irish movie, hit the heart strings</t>
+  </si>
+  <si>
+    <t>Pet Mart</t>
+  </si>
+  <si>
+    <t>Retail Associate</t>
+  </si>
+  <si>
+    <t>Direct Email</t>
+  </si>
+  <si>
+    <t>excellent movie. First I've seen with an intermission. As someone with an art history degree I really appreciated this. had to leave early had a dinner. Left at a really dark period of the movie</t>
   </si>
 </sst>
 </file>
@@ -3081,10 +3118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,6 +4226,54 @@
         <v>491</v>
       </c>
     </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B40" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>5</v>
+      </c>
+      <c r="K40" t="s">
+        <v>540</v>
+      </c>
+      <c r="L40" t="s">
+        <v>542</v>
+      </c>
+      <c r="M40" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>45663</v>
+      </c>
+      <c r="B41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4196,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4235,7 +4320,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>43423</v>
+        <v>45615</v>
       </c>
       <c r="B2" t="s">
         <v>388</v>
@@ -4264,7 +4349,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>43423</v>
+        <v>45615</v>
       </c>
       <c r="B3" t="s">
         <v>399</v>
@@ -4287,7 +4372,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>43424</v>
+        <v>45616</v>
       </c>
       <c r="B4" t="s">
         <v>404</v>
@@ -4307,7 +4392,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>43424</v>
+        <v>45616</v>
       </c>
       <c r="B5" t="s">
         <v>405</v>
@@ -4327,7 +4412,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>43424</v>
+        <v>45616</v>
       </c>
       <c r="B6" t="s">
         <v>410</v>
@@ -4347,7 +4432,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>43425</v>
+        <v>45617</v>
       </c>
       <c r="B7" t="s">
         <v>420</v>
@@ -4361,7 +4446,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>43425</v>
+        <v>45617</v>
       </c>
       <c r="B8" t="s">
         <v>423</v>
@@ -4381,7 +4466,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>43425</v>
+        <v>45617</v>
       </c>
       <c r="B9" t="s">
         <v>424</v>
@@ -4401,7 +4486,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>43425</v>
+        <v>45617</v>
       </c>
       <c r="B10" t="s">
         <v>428</v>
@@ -4421,7 +4506,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>43425</v>
+        <v>45617</v>
       </c>
       <c r="B11" t="s">
         <v>430</v>
@@ -4435,7 +4520,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>43431</v>
+        <v>45623</v>
       </c>
       <c r="B12" t="s">
         <v>450</v>
@@ -4461,7 +4546,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>43431</v>
+        <v>45623</v>
       </c>
       <c r="C13" t="s">
         <v>446</v>
@@ -4469,7 +4554,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>43431</v>
+        <v>45623</v>
       </c>
       <c r="B14" t="s">
         <v>451</v>
@@ -4483,7 +4568,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>43431</v>
+        <v>45623</v>
       </c>
       <c r="B15" t="s">
         <v>451</v>
@@ -4497,7 +4582,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>43431</v>
+        <v>45623</v>
       </c>
       <c r="B16" t="s">
         <v>404</v>
@@ -4508,7 +4593,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>43453</v>
+        <v>45645</v>
       </c>
       <c r="B17" t="s">
         <v>513</v>
@@ -4522,7 +4607,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>43460</v>
+        <v>45652</v>
       </c>
       <c r="B18" t="s">
         <v>451</v>
@@ -4542,7 +4627,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>43461</v>
+        <v>45653</v>
       </c>
       <c r="B19" t="s">
         <v>527</v>
@@ -4556,64 +4641,44 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>43464</v>
+        <v>45661</v>
       </c>
       <c r="B20" t="s">
+        <v>532</v>
+      </c>
+      <c r="C20" t="s">
         <v>533</v>
       </c>
-      <c r="C20" t="s">
-        <v>532</v>
-      </c>
       <c r="G20" t="s">
-        <v>535</v>
-      </c>
-      <c r="H20" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>43464</v>
+        <v>45661</v>
       </c>
       <c r="B21" t="s">
+        <v>535</v>
+      </c>
+      <c r="C21" t="s">
         <v>536</v>
       </c>
-      <c r="C21" t="s">
-        <v>537</v>
-      </c>
       <c r="G21" t="s">
-        <v>535</v>
-      </c>
-      <c r="H21" t="s">
-        <v>538</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>43464</v>
+        <v>45662</v>
       </c>
       <c r="B22" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="C22" t="s">
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="G22" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>43464</v>
-      </c>
-      <c r="B23" t="s">
-        <v>541</v>
-      </c>
-      <c r="C23" t="s">
-        <v>393</v>
-      </c>
-      <c r="G23" t="s">
-        <v>407</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -4622,6 +4687,76 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9354F74C-F7C9-484D-9594-9D8671DC07A9}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>538</v>
+      </c>
+      <c r="G1" t="s">
+        <v>539</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45660</v>
+      </c>
+      <c r="C2">
+        <v>7.6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>546</v>
+      </c>
+      <c r="E2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F2" t="s">
+        <v>545</v>
+      </c>
+      <c r="G2" t="s">
+        <v>544</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15FA9E0-547F-4AE8-9E5A-C35071F3E8D9}">
   <dimension ref="B2:N9"/>
   <sheetViews>
@@ -4966,10 +5101,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6198,6 +6333,52 @@
         <v>531</v>
       </c>
     </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B54" t="s">
+        <v>549</v>
+      </c>
+      <c r="C54">
+        <v>8.9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" t="s">
+        <v>87</v>
+      </c>
+      <c r="G54" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45661</v>
+      </c>
+      <c r="B55" t="s">
+        <v>548</v>
+      </c>
+      <c r="C55">
+        <v>8.1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" t="s">
+        <v>550</v>
+      </c>
+      <c r="G55" t="s">
+        <v>551</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6205,10 +6386,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6676,34 +6857,6 @@
         <v>516</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>542</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>439</v>
-      </c>
-      <c r="G21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>543</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>438</v>
-      </c>
-      <c r="G22" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6711,10 +6864,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7243,6 +7396,32 @@
       </c>
       <c r="H20" t="s">
         <v>504</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45660</v>
+      </c>
+      <c r="B21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C21">
+        <v>7.5</v>
+      </c>
+      <c r="D21">
+        <v>8.85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" t="s">
+        <v>547</v>
       </c>
     </row>
   </sheetData>
@@ -7481,7 +7660,7 @@
   <dimension ref="C5:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7876,7 +8055,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated for jan. 13, 2025
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFFA25F-47CA-4947-849F-EF266842997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2BD7F8-4379-41FB-B973-540A54FBEDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="1200" windowWidth="22155" windowHeight="11700" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="12105" yWindow="4950" windowWidth="22155" windowHeight="14130" activeTab="9" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="Concerts" sheetId="13" r:id="rId11"/>
     <sheet name="Dates" sheetId="9" state="hidden" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">'Job Aps'!$A$1:$G$58</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="613">
   <si>
     <t>Movie</t>
   </si>
@@ -1713,6 +1716,177 @@
   </si>
   <si>
     <t>excellent movie. First I've seen with an intermission. As someone with an art history degree I really appreciated this. had to leave early had a dinner. Left at a really dark period of the movie</t>
+  </si>
+  <si>
+    <t>Olli Brands</t>
+  </si>
+  <si>
+    <t>Cost Analyst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Analyst, Payment Decision Support </t>
+  </si>
+  <si>
+    <t>PC Financial</t>
+  </si>
+  <si>
+    <t>Direct workday</t>
+  </si>
+  <si>
+    <t>can wind up more</t>
+  </si>
+  <si>
+    <t>Caseware</t>
+  </si>
+  <si>
+    <t>Senior Data Analyst</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Business Intelligence Engineer</t>
+  </si>
+  <si>
+    <t>RAPS Consulting Inc</t>
+  </si>
+  <si>
+    <t>Landman</t>
+  </si>
+  <si>
+    <t>The Agency</t>
+  </si>
+  <si>
+    <t>Investment Analyst - Industrial Development – Transactions &amp; Acquistions</t>
+  </si>
+  <si>
+    <t>Beedie</t>
+  </si>
+  <si>
+    <t>Trade Analyst</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Alexandra Park</t>
+  </si>
+  <si>
+    <t>Blackout</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pretty cool indie wolfman movie not lame </t>
+  </si>
+  <si>
+    <t>got scored on first shift but turned it around. My passing was very good. Need to shoot more - one shift got 2 goals in a row on our end. Ended up winning 4-3</t>
+  </si>
+  <si>
+    <t>played outside for a hour before the ashl game. Pretty fun. Cold night</t>
+  </si>
+  <si>
+    <t>business analyst</t>
+  </si>
+  <si>
+    <t>EMBASSY GRAND CONVENTION CENTRE</t>
+  </si>
+  <si>
+    <t>Career Foundation</t>
+  </si>
+  <si>
+    <t>ASR INNOVATIONS INC</t>
+  </si>
+  <si>
+    <t>business systems specialist - computer systems</t>
+  </si>
+  <si>
+    <t>Missisauga</t>
+  </si>
+  <si>
+    <t>North York</t>
+  </si>
+  <si>
+    <t>Jamie XX</t>
+  </si>
+  <si>
+    <t>Conor</t>
+  </si>
+  <si>
+    <t>got me ticket for birthday?</t>
+  </si>
+  <si>
+    <t>AMW</t>
+  </si>
+  <si>
+    <t>not bad, better than I thought. Bonus for cheap</t>
+  </si>
+  <si>
+    <t>Bird</t>
+  </si>
+  <si>
+    <t>Weird, dark, and strange in that order. The bird thing surprised me and was sort of funny</t>
+  </si>
+  <si>
+    <t>shot a bit more but can do better</t>
+  </si>
+  <si>
+    <t>Hearts of Iron</t>
+  </si>
+  <si>
+    <t>Against the Storm</t>
+  </si>
+  <si>
+    <t>Monster</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Japanese</t>
+  </si>
+  <si>
+    <t>Squid Game</t>
+  </si>
+  <si>
+    <t>Indoor Etobicoke</t>
+  </si>
+  <si>
+    <t>Indoor Stockyards</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Saw at Kingsway. Had one person working on a Saturday night. Excellent movie, one of the best animations I've seen in a long time. No dialog</t>
+  </si>
+  <si>
+    <t>Thin Red Line</t>
+  </si>
+  <si>
+    <t>Action, Triller</t>
+  </si>
+  <si>
+    <t>Promising cast but fell flat. Enjoyable and will watch s2</t>
+  </si>
+  <si>
+    <t>Started strong, second half felt flat.</t>
+  </si>
+  <si>
+    <t>Progress Group Inc.</t>
+  </si>
+  <si>
+    <t>Oakville</t>
+  </si>
+  <si>
+    <t>Advisor Business Intelligence</t>
+  </si>
+  <si>
+    <t>Enbridge</t>
   </si>
 </sst>
 </file>
@@ -1723,10 +1897,26 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1740,7 +1930,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1748,19 +1938,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1846,7 +2139,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CA"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3118,10 +3411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4268,10 +4561,153 @@
       <c r="B41" t="s">
         <v>223</v>
       </c>
+      <c r="C41">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="K41" t="s">
+        <v>458</v>
+      </c>
+      <c r="M41" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45665</v>
+      </c>
       <c r="B42" t="s">
+        <v>573</v>
+      </c>
+      <c r="C42">
+        <v>8.1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="K42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45665</v>
+      </c>
+      <c r="B43" t="s">
         <v>224</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45667</v>
+      </c>
+      <c r="B44" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44">
+        <v>7.6</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="K44" t="s">
+        <v>458</v>
+      </c>
+      <c r="M44" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>45669</v>
+      </c>
+      <c r="B45" t="s">
+        <v>489</v>
+      </c>
+      <c r="C45">
+        <v>7.5</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45670</v>
+      </c>
+      <c r="B46" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4281,35 +4717,45 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="64" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="12" t="s">
         <v>402</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>572</v>
       </c>
       <c r="H1" t="s">
         <v>390</v>
@@ -4319,22 +4765,23 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="8">
         <v>45615</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="6" t="s">
         <v>407</v>
       </c>
       <c r="H2" t="s">
@@ -4348,19 +4795,21 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="10">
         <v>45615</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="7" t="s">
         <v>407</v>
       </c>
       <c r="H3" t="s">
@@ -4371,16 +4820,19 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="10">
         <v>45616</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="7" t="s">
         <v>408</v>
       </c>
       <c r="H4" t="s">
@@ -4391,16 +4843,19 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="10">
         <v>45616</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="G5" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="7" t="s">
         <v>408</v>
       </c>
       <c r="H5" t="s">
@@ -4411,16 +4866,19 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="10">
         <v>45616</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="7" t="s">
         <v>408</v>
       </c>
       <c r="H6" t="s">
@@ -4431,30 +4889,36 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="10">
         <v>45617</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="G7" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="7" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="10">
         <v>45617</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="G8" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="7" t="s">
         <v>408</v>
       </c>
       <c r="H8" t="s">
@@ -4465,16 +4929,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="10">
         <v>45617</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="G9" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="7" t="s">
         <v>408</v>
       </c>
       <c r="H9" t="s">
@@ -4485,16 +4952,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="10">
         <v>45617</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="G10" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="7" t="s">
         <v>407</v>
       </c>
       <c r="H10" t="s">
@@ -4505,39 +4975,43 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="10">
         <v>45617</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>431</v>
       </c>
-      <c r="G11" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="7" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="10">
         <v>45623</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="15" t="s">
         <v>444</v>
       </c>
       <c r="I12" t="s">
@@ -4545,77 +5019,100 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="10">
         <v>45623</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>446</v>
       </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="10">
         <v>45623</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="G14" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="7" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="10">
         <v>45623</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="G15" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="7" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="10">
         <v>45623</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>454</v>
       </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="10">
         <v>45645</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="11" t="s">
         <v>513</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11" t="s">
         <v>511</v>
       </c>
-      <c r="G17" t="s">
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="7" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="10">
         <v>45652</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="G18" t="s">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="7" t="s">
         <v>407</v>
       </c>
       <c r="H18" t="s">
@@ -4626,72 +5123,252 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="10">
         <v>45653</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="11" t="s">
         <v>527</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="11" t="s">
         <v>528</v>
       </c>
-      <c r="G19" t="s">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="7" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="10">
         <v>45661</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="11" t="s">
         <v>532</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>533</v>
       </c>
-      <c r="G20" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="7" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="10">
         <v>45661</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="11" t="s">
         <v>535</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>536</v>
       </c>
-      <c r="G21" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="7" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="10">
         <v>45662</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="11" t="s">
         <v>553</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="G22" t="s">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="7" t="s">
         <v>554</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>45663</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>45663</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>559</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="7" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>45664</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>45665</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>45665</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>45667</v>
+      </c>
+      <c r="B28" t="s">
+        <v>579</v>
+      </c>
+      <c r="C28" t="s">
+        <v>580</v>
+      </c>
+      <c r="F28" t="s">
+        <v>584</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>45667</v>
+      </c>
+      <c r="B29" t="s">
+        <v>583</v>
+      </c>
+      <c r="C29" t="s">
+        <v>582</v>
+      </c>
+      <c r="F29" t="s">
+        <v>585</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>45669</v>
+      </c>
+      <c r="B30" t="s">
+        <v>579</v>
+      </c>
+      <c r="C30" t="s">
+        <v>393</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>45670</v>
+      </c>
+      <c r="B31" t="s">
+        <v>423</v>
+      </c>
+      <c r="C31" t="s">
+        <v>609</v>
+      </c>
+      <c r="F31" t="s">
+        <v>610</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>45670</v>
+      </c>
+      <c r="B32" t="s">
+        <v>611</v>
+      </c>
+      <c r="C32" t="s">
+        <v>612</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H12" r:id="rId1" display="https://u16314525.ct.sendgrid.net/ls/click?upn=u001.arcBAojtThf9ZVITG3zqo-2B9n3nSRh67FlnXvXD6XiqJzD7CYRwHkblu9roGGB8aJXoneV-2By6QkQmXvCDRYC3Ow-3D-3DYURQ_viv87QBHgf3cZPYRGDRhIf5Ije2xX6iaAQx9P2mzXowwskAoPVVtw45JYM7FIvj8JBUA6fmZnC9NmVTrLulWtVMD-2FWr-2F7XVC8phWzOOKkZ9qlpxOCEUPara8dwPEtlufvt4WLgRxGI35qKXKtA5T8H9YCBVtvWElldCp8-2FCevr4VOiuZSBalYYKquYMyi0AFjalBv3D7Bp48pM4KUOzB0A-3D-3D" xr:uid="{32C2823C-8C79-43AB-9C1F-B592BF7964D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9354F74C-F7C9-484D-9594-9D8671DC07A9}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4749,6 +5426,23 @@
       </c>
       <c r="I2" t="s">
         <v>543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45671</v>
+      </c>
+      <c r="B3" t="s">
+        <v>586</v>
+      </c>
+      <c r="G3" t="s">
+        <v>587</v>
+      </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
+      <c r="I3" t="s">
+        <v>588</v>
       </c>
     </row>
   </sheetData>
@@ -5101,20 +5795,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5128,16 +5822,22 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>575</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>597</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45437</v>
       </c>
@@ -5150,17 +5850,17 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>87</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45439</v>
       </c>
@@ -5173,17 +5873,17 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>88</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45441</v>
       </c>
@@ -5196,17 +5896,17 @@
       <c r="D4" t="s">
         <v>145</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>49</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>89</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45448</v>
       </c>
@@ -5219,17 +5919,17 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>83</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>89</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45453</v>
       </c>
@@ -5242,17 +5942,17 @@
       <c r="D6" t="s">
         <v>143</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>49</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>89</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45454</v>
       </c>
@@ -5265,17 +5965,17 @@
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>83</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45455</v>
       </c>
@@ -5288,17 +5988,17 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>49</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>90</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45455</v>
       </c>
@@ -5311,17 +6011,17 @@
       <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>91</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45473</v>
       </c>
@@ -5334,17 +6034,17 @@
       <c r="D10" t="s">
         <v>85</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>87</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45476</v>
       </c>
@@ -5357,17 +6057,17 @@
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>89</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45483</v>
       </c>
@@ -5380,17 +6080,17 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>91</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45484</v>
       </c>
@@ -5403,17 +6103,17 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>87</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45486</v>
       </c>
@@ -5426,17 +6126,17 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>49</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>89</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45489</v>
       </c>
@@ -5449,17 +6149,17 @@
       <c r="D15" t="s">
         <v>120</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>89</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45490</v>
       </c>
@@ -5472,17 +6172,17 @@
       <c r="D16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>91</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45493</v>
       </c>
@@ -5495,17 +6195,17 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>89</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45497</v>
       </c>
@@ -5518,17 +6218,17 @@
       <c r="D18" t="s">
         <v>146</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>49</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>89</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45507</v>
       </c>
@@ -5541,17 +6241,17 @@
       <c r="D19" t="s">
         <v>85</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>83</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>91</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45488</v>
       </c>
@@ -5564,17 +6264,17 @@
       <c r="D20" t="s">
         <v>85</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>83</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>91</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45488</v>
       </c>
@@ -5587,17 +6287,17 @@
       <c r="D21" t="s">
         <v>10</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>83</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>91</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45483</v>
       </c>
@@ -5610,17 +6310,17 @@
       <c r="D22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>83</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>91</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45517</v>
       </c>
@@ -5633,17 +6333,17 @@
       <c r="D23" t="s">
         <v>10</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>49</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>91</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45521</v>
       </c>
@@ -5656,17 +6356,17 @@
       <c r="D24" t="s">
         <v>206</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>49</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>207</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45529</v>
       </c>
@@ -5679,17 +6379,17 @@
       <c r="D25" t="s">
         <v>213</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>49</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>212</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45530</v>
       </c>
@@ -5702,17 +6402,17 @@
       <c r="D26" t="s">
         <v>214</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>49</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>89</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45551</v>
       </c>
@@ -5725,17 +6425,17 @@
       <c r="D27" t="s">
         <v>11</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>49</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>231</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45556</v>
       </c>
@@ -5748,17 +6448,17 @@
       <c r="D28" t="s">
         <v>253</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>49</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>231</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45559</v>
       </c>
@@ -5771,17 +6471,17 @@
       <c r="D29" t="s">
         <v>266</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>49</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>231</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45564</v>
       </c>
@@ -5794,17 +6494,17 @@
       <c r="D30" t="s">
         <v>256</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>49</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>231</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45564</v>
       </c>
@@ -5817,17 +6517,17 @@
       <c r="D31" t="s">
         <v>10</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>83</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>231</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45566</v>
       </c>
@@ -5840,17 +6540,17 @@
       <c r="D32" t="s">
         <v>12</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>49</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>231</v>
       </c>
-      <c r="G32" t="s">
+      <c r="I32" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45570</v>
       </c>
@@ -5863,17 +6563,17 @@
       <c r="D33" t="s">
         <v>12</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>49</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>277</v>
       </c>
-      <c r="G33" t="s">
+      <c r="I33" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45574</v>
       </c>
@@ -5886,17 +6586,17 @@
       <c r="D34" t="s">
         <v>12</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>49</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>277</v>
       </c>
-      <c r="G34" t="s">
+      <c r="I34" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45574</v>
       </c>
@@ -5909,17 +6609,17 @@
       <c r="D35" t="s">
         <v>12</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>49</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>277</v>
       </c>
-      <c r="G35" t="s">
+      <c r="I35" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45575</v>
       </c>
@@ -5932,17 +6632,17 @@
       <c r="D36" t="s">
         <v>12</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>49</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>277</v>
       </c>
-      <c r="G36" t="s">
+      <c r="I36" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45578</v>
       </c>
@@ -5955,17 +6655,17 @@
       <c r="D37" t="s">
         <v>100</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>49</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>231</v>
       </c>
-      <c r="G37" t="s">
+      <c r="I37" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45585</v>
       </c>
@@ -5978,17 +6678,17 @@
       <c r="D38" t="s">
         <v>297</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>49</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>300</v>
       </c>
-      <c r="G38" t="s">
+      <c r="I38" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45585</v>
       </c>
@@ -6001,17 +6701,17 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>49</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>300</v>
       </c>
-      <c r="G39" t="s">
+      <c r="I39" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45587</v>
       </c>
@@ -6024,17 +6724,17 @@
       <c r="D40" t="s">
         <v>12</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>49</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>318</v>
       </c>
-      <c r="G40" t="s">
+      <c r="I40" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45584</v>
       </c>
@@ -6047,17 +6747,17 @@
       <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>49</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>231</v>
       </c>
-      <c r="G41" t="s">
+      <c r="I41" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45610</v>
       </c>
@@ -6070,17 +6770,17 @@
       <c r="D42" t="s">
         <v>373</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>83</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>300</v>
       </c>
-      <c r="G42" t="s">
+      <c r="I42" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45624</v>
       </c>
@@ -6093,17 +6793,17 @@
       <c r="D43" t="s">
         <v>456</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>49</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>87</v>
       </c>
-      <c r="G43" t="s">
+      <c r="I43" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45638</v>
       </c>
@@ -6116,17 +6816,17 @@
       <c r="D44" t="s">
         <v>466</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>49</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>91</v>
       </c>
-      <c r="G44" t="s">
+      <c r="I44" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45633</v>
       </c>
@@ -6139,17 +6839,17 @@
       <c r="D45" t="s">
         <v>11</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>49</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>231</v>
       </c>
-      <c r="G45" t="s">
+      <c r="I45" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45635</v>
       </c>
@@ -6162,17 +6862,17 @@
       <c r="D46" t="s">
         <v>11</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>49</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>231</v>
       </c>
-      <c r="G46" t="s">
+      <c r="I46" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45638</v>
       </c>
@@ -6185,17 +6885,17 @@
       <c r="D47" t="s">
         <v>502</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>49</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>300</v>
       </c>
-      <c r="G47" t="s">
+      <c r="I47" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45640</v>
       </c>
@@ -6208,17 +6908,17 @@
       <c r="D48" t="s">
         <v>100</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>49</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>300</v>
       </c>
-      <c r="G48" t="s">
+      <c r="I48" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45641</v>
       </c>
@@ -6231,17 +6931,17 @@
       <c r="D49" t="s">
         <v>214</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>49</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>300</v>
       </c>
-      <c r="G49" t="s">
+      <c r="I49" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45643</v>
       </c>
@@ -6254,17 +6954,17 @@
       <c r="D50" t="s">
         <v>509</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>49</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>91</v>
       </c>
-      <c r="G50" t="s">
+      <c r="I50" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45647</v>
       </c>
@@ -6277,17 +6977,17 @@
       <c r="D51" t="s">
         <v>214</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>49</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>91</v>
       </c>
-      <c r="G51" t="s">
+      <c r="I51" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45648</v>
       </c>
@@ -6300,17 +7000,17 @@
       <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>49</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>91</v>
       </c>
-      <c r="G52" t="s">
+      <c r="I52" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45653</v>
       </c>
@@ -6323,17 +7023,17 @@
       <c r="D53" t="s">
         <v>530</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>49</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>87</v>
       </c>
-      <c r="G53" t="s">
+      <c r="I53" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45660</v>
       </c>
@@ -6346,17 +7046,17 @@
       <c r="D54" t="s">
         <v>11</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>83</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>87</v>
       </c>
-      <c r="G54" t="s">
+      <c r="I54" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45661</v>
       </c>
@@ -6369,14 +7069,123 @@
       <c r="D55" t="s">
         <v>11</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>49</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>550</v>
       </c>
-      <c r="G55" t="s">
+      <c r="I55" t="s">
         <v>551</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>45666</v>
+      </c>
+      <c r="B56" t="s">
+        <v>574</v>
+      </c>
+      <c r="C56">
+        <v>7.1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>530</v>
+      </c>
+      <c r="E56">
+        <v>2023</v>
+      </c>
+      <c r="F56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" t="s">
+        <v>550</v>
+      </c>
+      <c r="I56" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>45667</v>
+      </c>
+      <c r="B57" t="s">
+        <v>591</v>
+      </c>
+      <c r="C57">
+        <v>7.3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57">
+        <v>2024</v>
+      </c>
+      <c r="F57" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" t="s">
+        <v>550</v>
+      </c>
+      <c r="I57" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>45668</v>
+      </c>
+      <c r="B58" t="s">
+        <v>602</v>
+      </c>
+      <c r="C58">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D58" t="s">
+        <v>603</v>
+      </c>
+      <c r="E58">
+        <v>2024</v>
+      </c>
+      <c r="F58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G58" t="s">
+        <v>87</v>
+      </c>
+      <c r="I58" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>45669</v>
+      </c>
+      <c r="B59" t="s">
+        <v>596</v>
+      </c>
+      <c r="C59">
+        <v>7.1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59">
+        <v>2023</v>
+      </c>
+      <c r="G59" t="s">
+        <v>442</v>
+      </c>
+      <c r="H59" t="s">
+        <v>598</v>
+      </c>
+      <c r="I59" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -6386,10 +7195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6739,6 +7548,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45653</v>
+      </c>
       <c r="B14" t="s">
         <v>432</v>
       </c>
@@ -6746,13 +7558,16 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>7.6</v>
       </c>
       <c r="E14" t="s">
         <v>49</v>
       </c>
       <c r="F14" t="s">
         <v>438</v>
+      </c>
+      <c r="G14" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6855,6 +7670,51 @@
       </c>
       <c r="H20" t="s">
         <v>516</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45670</v>
+      </c>
+      <c r="B21" t="s">
+        <v>567</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>7.1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>438</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45665</v>
+      </c>
+      <c r="B23" t="s">
+        <v>599</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>7.3</v>
       </c>
     </row>
   </sheetData>
@@ -6864,10 +7724,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7424,6 +8284,32 @@
         <v>547</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45667</v>
+      </c>
+      <c r="B22" t="s">
+        <v>589</v>
+      </c>
+      <c r="C22">
+        <v>6.9</v>
+      </c>
+      <c r="D22">
+        <v>6.85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" t="s">
+        <v>590</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7431,10 +8317,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9CAB6AD-E088-49BC-A679-AC7F288052E6}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD3"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7650,6 +8536,16 @@
         <v>347</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>595</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7660,7 +8556,7 @@
   <dimension ref="C5:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8052,10 +8948,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C618A1B-BDBF-4797-B662-4C6D10CA0F5E}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8285,6 +9181,22 @@
       </c>
       <c r="K8" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>600</v>
+      </c>
+      <c r="C9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>45670</v>
+      </c>
+      <c r="B10" t="s">
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for week of jan 27, 2025
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2BD7F8-4379-41FB-B973-540A54FBEDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B7C148-7725-4392-90F8-109AD12E391B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12105" yWindow="4950" windowWidth="22155" windowHeight="14130" activeTab="9" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Dates" sheetId="9" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="9">'Job Aps'!$A$1:$G$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">'Job Aps'!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="677">
   <si>
     <t>Movie</t>
   </si>
@@ -1700,9 +1700,6 @@
     <t>Brutalist</t>
   </si>
   <si>
-    <t>Steam</t>
-  </si>
-  <si>
     <t>solid irish movie, hit the heart strings</t>
   </si>
   <si>
@@ -1814,9 +1811,6 @@
     <t>Conor</t>
   </si>
   <si>
-    <t>got me ticket for birthday?</t>
-  </si>
-  <si>
     <t>AMW</t>
   </si>
   <si>
@@ -1887,6 +1881,204 @@
   </si>
   <si>
     <t>Enbridge</t>
+  </si>
+  <si>
+    <t>War</t>
+  </si>
+  <si>
+    <t>It was alright, nick nolte was very good. The hill scene was interesting. Not the best war movie ive ever seen.</t>
+  </si>
+  <si>
+    <t>Data Engineer I</t>
+  </si>
+  <si>
+    <t>Coalition</t>
+  </si>
+  <si>
+    <t>posted 2 weeks ago unlikely</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intelligence Analyst - Various positions </t>
+  </si>
+  <si>
+    <t>Gov Canada</t>
+  </si>
+  <si>
+    <t>emailed directly - https://emploisfp-psjobs.cfp-psc.gc.ca/psrs-srfp/applicant/page1800?poster=2264579</t>
+  </si>
+  <si>
+    <t>Business Data Analyst</t>
+  </si>
+  <si>
+    <t>The Mirillion Group</t>
+  </si>
+  <si>
+    <t>Data Engineer</t>
+  </si>
+  <si>
+    <t>Business Systems Analyst</t>
+  </si>
+  <si>
+    <t>didn’t work</t>
+  </si>
+  <si>
+    <t>Business System Analyst</t>
+  </si>
+  <si>
+    <t>Bank of Canada</t>
+  </si>
+  <si>
+    <t>Analyst, Cyber Security Awareness</t>
+  </si>
+  <si>
+    <t>Junior Data Scientist</t>
+  </si>
+  <si>
+    <t>closed 16-01-25 and results available 06-04</t>
+  </si>
+  <si>
+    <t>was a good game</t>
+  </si>
+  <si>
+    <t>fun time, need to dyke in more</t>
+  </si>
+  <si>
+    <t>11:15 pm game was kind of tired, felt like I had brick hands and couldn’t move that fast. Good game though, we won 5-4 with 8 guys</t>
+  </si>
+  <si>
+    <t>Incendies</t>
+  </si>
+  <si>
+    <t>No Where</t>
+  </si>
+  <si>
+    <t>Abigale</t>
+  </si>
+  <si>
+    <t>Electronic</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Visibility</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>got me ticket as present. We enjoyed it but had short people problems and couldn't see mnuch in the pit. Was unimpressed by the lack of effort, no bands or instruments or anything special. Won't go see DJ's like this again.</t>
+  </si>
+  <si>
+    <t>Toshi, Chris, Spencer</t>
+  </si>
+  <si>
+    <t>Suspiria.2018</t>
+  </si>
+  <si>
+    <t>A.Real.Pain.2024</t>
+  </si>
+  <si>
+    <t>enjoyed it until the middle and it got increasingly strange and I was confused</t>
+  </si>
+  <si>
+    <t>great film. Funny, weird, and to the heart. Cast was awesome</t>
+  </si>
+  <si>
+    <t>Watchmen Chapter 1</t>
+  </si>
+  <si>
+    <t>Watchmen Chapter 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Den of Thieves 2 </t>
+  </si>
+  <si>
+    <t>Drama/Action</t>
+  </si>
+  <si>
+    <t>it was good, disliked the ending</t>
+  </si>
+  <si>
+    <t>Sniper: Inside the Crosshairs</t>
+  </si>
+  <si>
+    <t>interesting. Canadian had the furthest shot ever!</t>
+  </si>
+  <si>
+    <t>Carriers</t>
+  </si>
+  <si>
+    <t>Thriller/Drama</t>
+  </si>
+  <si>
+    <t>good effort. Not very good. Sudden ending, not enjoyable</t>
+  </si>
+  <si>
+    <t>A Midnight Clear</t>
+  </si>
+  <si>
+    <t>one of the strangest ww2 movies ive seen. Enjoyed it</t>
+  </si>
+  <si>
+    <t>stream</t>
+  </si>
+  <si>
+    <t>War/Drama</t>
+  </si>
+  <si>
+    <t>The Order</t>
+  </si>
+  <si>
+    <t>very good. Interesting a disturbing true story. Mark maron was great</t>
+  </si>
+  <si>
+    <t>Get Away</t>
+  </si>
+  <si>
+    <t>I like nick frost and aisling bea but this movie wasn’t that good. Decent twist though</t>
+  </si>
+  <si>
+    <t>Queer</t>
+  </si>
+  <si>
+    <t>We Own the night</t>
+  </si>
+  <si>
+    <t>Very good - occurred prior to 2017 when trump took over. In depth look at what happened, I didn't know the story. Great acting all around with some from Wire making another appearance.</t>
+  </si>
+  <si>
+    <t>Donatellis</t>
+  </si>
+  <si>
+    <t>they call it an "English Poutine", I did not think it was very good and tasted kind of burnt. Decent value though and price. Only got it because I had no cash for apache.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Insights Analyst </t>
+  </si>
+  <si>
+    <t>Air Canada</t>
+  </si>
+  <si>
+    <t>probably need to be bilingual but lets see</t>
+  </si>
+  <si>
+    <t>new resume template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEALTH INFORMATION ANALYST </t>
+  </si>
+  <si>
+    <t>good game was just a little slow and tired</t>
+  </si>
+  <si>
+    <t>fun game I think I played well and beautiful day</t>
+  </si>
+  <si>
+    <t>played great. Felt good</t>
+  </si>
+  <si>
+    <t>couple good guys on the other team. I think I played well but had a bit of a cold. We were short a guy too pretty tired</t>
   </si>
 </sst>
 </file>
@@ -2049,8 +2241,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3411,10 +3603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4583,7 +4775,7 @@
         <v>458</v>
       </c>
       <c r="M41" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -4591,7 +4783,7 @@
         <v>45665</v>
       </c>
       <c r="B42" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C42">
         <v>8.1</v>
@@ -4612,7 +4804,7 @@
         <v>6</v>
       </c>
       <c r="K42" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -4641,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -4673,7 +4865,7 @@
         <v>458</v>
       </c>
       <c r="M44" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -4701,6 +4893,9 @@
       <c r="H45">
         <v>3</v>
       </c>
+      <c r="M45" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -4708,6 +4903,154 @@
       </c>
       <c r="B46" t="s">
         <v>223</v>
+      </c>
+      <c r="C46">
+        <v>8.1</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="M46" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45672</v>
+      </c>
+      <c r="B47" t="s">
+        <v>224</v>
+      </c>
+      <c r="C47">
+        <v>7.1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="M47" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C48">
+        <v>8.4</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="M48" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45676</v>
+      </c>
+      <c r="B49" t="s">
+        <v>489</v>
+      </c>
+      <c r="C49">
+        <v>7.5</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="M49" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45683</v>
+      </c>
+      <c r="B50" t="s">
+        <v>489</v>
+      </c>
+      <c r="C50">
+        <v>7.9</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="M50" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45684</v>
+      </c>
+      <c r="B51" t="s">
+        <v>223</v>
+      </c>
+      <c r="C51">
+        <v>7.8</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="M51" t="s">
+        <v>676</v>
       </c>
     </row>
   </sheetData>
@@ -4717,10 +5060,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4755,7 +5098,7 @@
         <v>402</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H1" t="s">
         <v>390</v>
@@ -5011,7 +5354,7 @@
       <c r="G12" s="7" t="s">
         <v>445</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>444</v>
       </c>
       <c r="I12" t="s">
@@ -5023,7 +5366,7 @@
         <v>45623</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>446</v>
@@ -5178,16 +5521,16 @@
         <v>45662</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="7" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5195,10 +5538,10 @@
         <v>45663</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
@@ -5212,16 +5555,16 @@
         <v>45663</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>557</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>558</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>559</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="7" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -5229,16 +5572,16 @@
         <v>45664</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5246,10 +5589,10 @@
         <v>45665</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>564</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>565</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>566</v>
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
@@ -5263,16 +5606,16 @@
         <v>45665</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>568</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>569</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>570</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -5280,16 +5623,16 @@
         <v>45667</v>
       </c>
       <c r="B28" t="s">
+        <v>578</v>
+      </c>
+      <c r="C28" t="s">
         <v>579</v>
       </c>
-      <c r="C28" t="s">
+      <c r="F28" t="s">
+        <v>583</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>580</v>
-      </c>
-      <c r="F28" t="s">
-        <v>584</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5297,16 +5640,16 @@
         <v>45667</v>
       </c>
       <c r="B29" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C29" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -5314,13 +5657,13 @@
         <v>45669</v>
       </c>
       <c r="B30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C30" t="s">
         <v>393</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -5331,12 +5674,12 @@
         <v>423</v>
       </c>
       <c r="C31" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F31" t="s">
-        <v>610</v>
-      </c>
-      <c r="G31" s="14" t="s">
+        <v>608</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>408</v>
       </c>
     </row>
@@ -5345,13 +5688,165 @@
         <v>45670</v>
       </c>
       <c r="B32" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C32" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B33" t="s">
+        <v>613</v>
+      </c>
+      <c r="C33" t="s">
+        <v>614</v>
+      </c>
+      <c r="F33" t="s">
+        <v>615</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B34" t="s">
+        <v>619</v>
+      </c>
+      <c r="C34" t="s">
+        <v>620</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B35" t="s">
+        <v>621</v>
+      </c>
+      <c r="C35" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B36" t="s">
+        <v>616</v>
+      </c>
+      <c r="C36" t="s">
+        <v>617</v>
+      </c>
+      <c r="E36" t="s">
+        <v>623</v>
+      </c>
+      <c r="F36" t="s">
+        <v>618</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B37" t="s">
+        <v>622</v>
+      </c>
+      <c r="C37" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B38" t="s">
+        <v>624</v>
+      </c>
+      <c r="C38" t="s">
+        <v>625</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B39" t="s">
+        <v>626</v>
+      </c>
+      <c r="C39" t="s">
+        <v>625</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B40" t="s">
+        <v>627</v>
+      </c>
+      <c r="C40" t="s">
+        <v>617</v>
+      </c>
+      <c r="F40" t="s">
+        <v>628</v>
+      </c>
+      <c r="G40" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>45681</v>
+      </c>
+      <c r="B41" t="s">
+        <v>672</v>
+      </c>
+      <c r="C41" t="s">
+        <v>421</v>
+      </c>
+      <c r="F41" t="s">
+        <v>671</v>
+      </c>
+      <c r="G41" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>45684</v>
+      </c>
+      <c r="B42" t="s">
+        <v>668</v>
+      </c>
+      <c r="C42" t="s">
+        <v>669</v>
+      </c>
+      <c r="F42" t="s">
+        <v>670</v>
+      </c>
+      <c r="G42" t="s">
+        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -5365,15 +5860,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9354F74C-F7C9-484D-9594-9D8671DC07A9}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5393,16 +5888,22 @@
         <v>538</v>
       </c>
       <c r="G1" t="s">
+        <v>637</v>
+      </c>
+      <c r="H1" t="s">
+        <v>638</v>
+      </c>
+      <c r="I1" t="s">
         <v>539</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45660</v>
       </c>
@@ -5418,31 +5919,55 @@
       <c r="F2" t="s">
         <v>545</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.4</v>
+      </c>
+      <c r="I2" t="s">
         <v>544</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45671</v>
       </c>
       <c r="B3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C3">
+        <v>7.7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>635</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>636</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="I3" t="s">
         <v>586</v>
       </c>
-      <c r="G3" t="s">
-        <v>587</v>
-      </c>
-      <c r="H3">
-        <v>45</v>
-      </c>
-      <c r="I3" t="s">
-        <v>588</v>
+      <c r="J3">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -5795,10 +6320,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5822,7 +6347,7 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -5831,7 +6356,7 @@
         <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -7053,7 +7578,7 @@
         <v>87</v>
       </c>
       <c r="I54" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -7073,10 +7598,10 @@
         <v>49</v>
       </c>
       <c r="G55" t="s">
+        <v>300</v>
+      </c>
+      <c r="I55" t="s">
         <v>550</v>
-      </c>
-      <c r="I55" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -7084,7 +7609,7 @@
         <v>45666</v>
       </c>
       <c r="B56" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C56">
         <v>7.1</v>
@@ -7099,10 +7624,10 @@
         <v>49</v>
       </c>
       <c r="G56" t="s">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="I56" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -7110,7 +7635,7 @@
         <v>45667</v>
       </c>
       <c r="B57" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C57">
         <v>7.3</v>
@@ -7125,10 +7650,10 @@
         <v>49</v>
       </c>
       <c r="G57" t="s">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="I57" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -7136,13 +7661,13 @@
         <v>45668</v>
       </c>
       <c r="B58" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C58">
         <v>9.3000000000000007</v>
       </c>
       <c r="D58" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E58">
         <v>2024</v>
@@ -7154,7 +7679,7 @@
         <v>87</v>
       </c>
       <c r="I58" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -7162,7 +7687,7 @@
         <v>45669</v>
       </c>
       <c r="B59" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C59">
         <v>7.1</v>
@@ -7173,19 +7698,312 @@
       <c r="E59">
         <v>2023</v>
       </c>
+      <c r="F59" t="s">
+        <v>49</v>
+      </c>
       <c r="G59" t="s">
         <v>442</v>
       </c>
       <c r="H59" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I59" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>45671</v>
+      </c>
       <c r="B60" t="s">
-        <v>605</v>
+        <v>603</v>
+      </c>
+      <c r="C60">
+        <v>7.2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>611</v>
+      </c>
+      <c r="E60">
+        <v>1998</v>
+      </c>
+      <c r="F60" t="s">
+        <v>49</v>
+      </c>
+      <c r="G60" t="s">
+        <v>231</v>
+      </c>
+      <c r="I60" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" t="s">
+        <v>632</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61">
+        <v>2010</v>
+      </c>
+      <c r="G61" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>633</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62">
+        <v>2023</v>
+      </c>
+      <c r="G62" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>634</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <v>2023</v>
+      </c>
+      <c r="G63" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B64" t="s">
+        <v>641</v>
+      </c>
+      <c r="C64">
+        <v>6.8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G64" t="s">
+        <v>231</v>
+      </c>
+      <c r="I64" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>45673</v>
+      </c>
+      <c r="B65" t="s">
+        <v>642</v>
+      </c>
+      <c r="C65">
+        <v>8.1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>100</v>
+      </c>
+      <c r="F65" t="s">
+        <v>49</v>
+      </c>
+      <c r="G65" t="s">
+        <v>231</v>
+      </c>
+      <c r="I65" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45674</v>
+      </c>
+      <c r="B68" t="s">
+        <v>647</v>
+      </c>
+      <c r="C68">
+        <v>7.2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>648</v>
+      </c>
+      <c r="E68">
+        <v>2025</v>
+      </c>
+      <c r="F68" t="s">
+        <v>49</v>
+      </c>
+      <c r="G68" t="s">
+        <v>231</v>
+      </c>
+      <c r="I68" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>45670</v>
+      </c>
+      <c r="B69" t="s">
+        <v>650</v>
+      </c>
+      <c r="C69">
+        <v>7.6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>120</v>
+      </c>
+      <c r="F69" t="s">
+        <v>49</v>
+      </c>
+      <c r="G69" t="s">
+        <v>231</v>
+      </c>
+      <c r="I69" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B70" t="s">
+        <v>652</v>
+      </c>
+      <c r="C70">
+        <v>6.8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>653</v>
+      </c>
+      <c r="E70">
+        <v>2009</v>
+      </c>
+      <c r="F70" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70" t="s">
+        <v>91</v>
+      </c>
+      <c r="I70" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B71" t="s">
+        <v>655</v>
+      </c>
+      <c r="C71">
+        <v>7.7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>658</v>
+      </c>
+      <c r="E71">
+        <v>1992</v>
+      </c>
+      <c r="G71" t="s">
+        <v>657</v>
+      </c>
+      <c r="I71" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45677</v>
+      </c>
+      <c r="B72" t="s">
+        <v>659</v>
+      </c>
+      <c r="C72">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>653</v>
+      </c>
+      <c r="E72">
+        <v>2024</v>
+      </c>
+      <c r="F72" t="s">
+        <v>49</v>
+      </c>
+      <c r="G72" t="s">
+        <v>231</v>
+      </c>
+      <c r="I72" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>45678</v>
+      </c>
+      <c r="B73" t="s">
+        <v>661</v>
+      </c>
+      <c r="C73">
+        <v>6.7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73">
+        <v>2024</v>
+      </c>
+      <c r="F73" t="s">
+        <v>49</v>
+      </c>
+      <c r="G73" t="s">
+        <v>231</v>
+      </c>
+      <c r="I73" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>45678</v>
+      </c>
+      <c r="B74" t="s">
+        <v>663</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74">
+        <v>2024</v>
+      </c>
+      <c r="F74" t="s">
+        <v>49</v>
+      </c>
+      <c r="G74" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -7195,10 +8013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7567,7 +8385,7 @@
         <v>438</v>
       </c>
       <c r="G14" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -7677,7 +8495,7 @@
         <v>45670</v>
       </c>
       <c r="B21" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -7695,12 +8513,12 @@
         <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -7708,13 +8526,39 @@
         <v>45665</v>
       </c>
       <c r="B23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
         <v>7.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B24" t="s">
+        <v>664</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" t="s">
+        <v>442</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" t="s">
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -7724,10 +8568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8289,7 +9133,7 @@
         <v>45667</v>
       </c>
       <c r="B22" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C22">
         <v>6.9</v>
@@ -8307,7 +9151,33 @@
         <v>96</v>
       </c>
       <c r="H22" t="s">
-        <v>590</v>
+        <v>588</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45680</v>
+      </c>
+      <c r="B23" t="s">
+        <v>666</v>
+      </c>
+      <c r="C23">
+        <v>6.9</v>
+      </c>
+      <c r="D23">
+        <v>8.5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" t="s">
+        <v>667</v>
       </c>
     </row>
   </sheetData>
@@ -8538,12 +9408,12 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -8951,7 +9821,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9185,7 +10055,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C9">
         <v>93</v>
@@ -9196,7 +10066,16 @@
         <v>45670</v>
       </c>
       <c r="B10" t="s">
-        <v>601</v>
+        <v>599</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -9210,7 +10089,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated for week of feb 10th
</commit_message>
<xml_diff>
--- a/20241108  - Data Science Personal Log.xlsx
+++ b/20241108  - Data Science Personal Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B7C148-7725-4392-90F8-109AD12E391B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E562F478-E544-460E-A7DD-F58B5D85BD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
+    <workbookView xWindow="15960" yWindow="1425" windowWidth="19455" windowHeight="14850" xr2:uid="{232BB0B9-F4C5-4BA7-ACF9-8C60FC565B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hockey" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'Job Aps'!$A$1:$G$56</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="726">
   <si>
     <t>Movie</t>
   </si>
@@ -2079,6 +2079,153 @@
   </si>
   <si>
     <t>couple good guys on the other team. I think I played well but had a bit of a cold. We were short a guy too pretty tired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financial Analyst </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ministry of the Attorney General </t>
+  </si>
+  <si>
+    <t>Humane</t>
+  </si>
+  <si>
+    <t>Uline</t>
+  </si>
+  <si>
+    <t>OMERS/Oxford Properties</t>
+  </si>
+  <si>
+    <t>ata Engineer (Data Visualization and Analytics)</t>
+  </si>
+  <si>
+    <t>was ok. Lost interest when they went tripping</t>
+  </si>
+  <si>
+    <t>Babygirl</t>
+  </si>
+  <si>
+    <t>decent movie. I had a hard time connecting with the male lead</t>
+  </si>
+  <si>
+    <t>pretty good Canadian movie. Enjoyed it. You can sacrifice yourself to the gov' for $250K</t>
+  </si>
+  <si>
+    <t>2 thumbs up - good stuff</t>
+  </si>
+  <si>
+    <t>we lost 5-3 and they scored 4 connsective goals, 2-3 of which were on me. But I got the player of the game so I must have done well elsewhere</t>
+  </si>
+  <si>
+    <t>passing</t>
+  </si>
+  <si>
+    <t>shot - get it up! Not on the ice from the point</t>
+  </si>
+  <si>
+    <t>defence</t>
+  </si>
+  <si>
+    <t>Policy and Planning Advisor (10418)</t>
+  </si>
+  <si>
+    <t>TTC</t>
+  </si>
+  <si>
+    <t>OCS</t>
+  </si>
+  <si>
+    <t>Business Transformation Analyst</t>
+  </si>
+  <si>
+    <t>Harveys</t>
+  </si>
+  <si>
+    <t>with  onion ring</t>
+  </si>
+  <si>
+    <t>not good</t>
+  </si>
+  <si>
+    <t>On Call</t>
+  </si>
+  <si>
+    <t>Paradise</t>
+  </si>
+  <si>
+    <t>The killing</t>
+  </si>
+  <si>
+    <t>great book, well researched and written. Learned a lot</t>
+  </si>
+  <si>
+    <t>was hungover so played back. Played ok</t>
+  </si>
+  <si>
+    <t>passing and stick handling not bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business &amp; Financial Analyst (Asset Management Specialist) </t>
+  </si>
+  <si>
+    <t>played almost whole game was fun. Slow but fun</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>She Said</t>
+  </si>
+  <si>
+    <t>Woman of the Hour</t>
+  </si>
+  <si>
+    <t>good movie, enjoyed it. Fun trump scene. Is the winstein voice vince vaughn?</t>
+  </si>
+  <si>
+    <t>Financial Data Analyst</t>
+  </si>
+  <si>
+    <t>Paymentus</t>
+  </si>
+  <si>
+    <t>Data Analyst (Power BI/SQL Developer)</t>
+  </si>
+  <si>
+    <t>Sales Operations Analyst</t>
+  </si>
+  <si>
+    <t>Achievers</t>
+  </si>
+  <si>
+    <t>It was ok. Bit all over the place. Enjoyable - will continue</t>
+  </si>
+  <si>
+    <t>light on the fries but still good. Maybe for future orders buy with side of gravy and do the cheese at home</t>
+  </si>
+  <si>
+    <t>6pm</t>
+  </si>
+  <si>
+    <t>played maybe 90% of the game. So tired. Somehow we won</t>
+  </si>
+  <si>
+    <t>Analytics Engineer</t>
+  </si>
+  <si>
+    <t>KUBRA</t>
+  </si>
+  <si>
+    <t>Business Intelligence Data Analyst</t>
+  </si>
+  <si>
+    <t>Shein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HearingLife </t>
+  </si>
+  <si>
+    <t>sent to carina directly no CL required</t>
   </si>
 </sst>
 </file>
@@ -2226,7 +2373,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2243,6 +2390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3603,10 +3751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0EEF53-D952-4518-BEAE-105433A5CF94}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5049,9 +5197,146 @@
       <c r="F51">
         <v>1</v>
       </c>
+      <c r="K51" t="s">
+        <v>691</v>
+      </c>
       <c r="M51" t="s">
         <v>676</v>
       </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>45686</v>
+      </c>
+      <c r="B52" t="s">
+        <v>224</v>
+      </c>
+      <c r="C52">
+        <v>7.8</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>-2</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="K52" t="s">
+        <v>689</v>
+      </c>
+      <c r="L52" t="s">
+        <v>690</v>
+      </c>
+      <c r="M52" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B53" t="s">
+        <v>489</v>
+      </c>
+      <c r="C53">
+        <v>7.7</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="K53" t="s">
+        <v>704</v>
+      </c>
+      <c r="M53" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B54" t="s">
+        <v>223</v>
+      </c>
+      <c r="C54">
+        <v>7.9</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
+      <c r="K54" t="s">
+        <v>689</v>
+      </c>
+      <c r="L54" t="s">
+        <v>707</v>
+      </c>
+      <c r="M54" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45698</v>
+      </c>
+      <c r="B55" t="s">
+        <v>223</v>
+      </c>
+      <c r="C55">
+        <v>7.7</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="M55" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5060,10 +5345,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3FCBAF-CC3B-454E-93B9-7B5151BEC9AC}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5847,6 +6132,180 @@
       </c>
       <c r="G42" t="s">
         <v>563</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>45685</v>
+      </c>
+      <c r="B43" t="s">
+        <v>677</v>
+      </c>
+      <c r="C43" t="s">
+        <v>678</v>
+      </c>
+      <c r="F43" t="s">
+        <v>671</v>
+      </c>
+      <c r="G43" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>45686</v>
+      </c>
+      <c r="B44" t="s">
+        <v>535</v>
+      </c>
+      <c r="C44" t="s">
+        <v>680</v>
+      </c>
+      <c r="G44" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>45687</v>
+      </c>
+      <c r="B45" t="s">
+        <v>682</v>
+      </c>
+      <c r="C45" t="s">
+        <v>681</v>
+      </c>
+      <c r="G45" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>45688</v>
+      </c>
+      <c r="B46" t="s">
+        <v>692</v>
+      </c>
+      <c r="C46" t="s">
+        <v>693</v>
+      </c>
+      <c r="G46" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>45688</v>
+      </c>
+      <c r="B47" t="s">
+        <v>695</v>
+      </c>
+      <c r="C47" t="s">
+        <v>694</v>
+      </c>
+      <c r="G47" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>45690</v>
+      </c>
+      <c r="B48" t="s">
+        <v>705</v>
+      </c>
+      <c r="C48" t="s">
+        <v>421</v>
+      </c>
+      <c r="G48" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>45692</v>
+      </c>
+      <c r="B49" t="s">
+        <v>711</v>
+      </c>
+      <c r="C49" t="s">
+        <v>712</v>
+      </c>
+      <c r="G49" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>45692</v>
+      </c>
+      <c r="B50" t="s">
+        <v>713</v>
+      </c>
+      <c r="C50" t="s">
+        <v>681</v>
+      </c>
+      <c r="G50" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>45694</v>
+      </c>
+      <c r="B51" t="s">
+        <v>714</v>
+      </c>
+      <c r="C51" t="s">
+        <v>715</v>
+      </c>
+      <c r="G51" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>45699</v>
+      </c>
+      <c r="B52" t="s">
+        <v>720</v>
+      </c>
+      <c r="C52" t="s">
+        <v>721</v>
+      </c>
+      <c r="G52" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>45699</v>
+      </c>
+      <c r="B53" t="s">
+        <v>722</v>
+      </c>
+      <c r="C53" t="s">
+        <v>724</v>
+      </c>
+      <c r="E53" t="s">
+        <v>725</v>
+      </c>
+      <c r="G53" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>45699</v>
+      </c>
+      <c r="B54" t="s">
+        <v>451</v>
+      </c>
+      <c r="C54" t="s">
+        <v>723</v>
+      </c>
+      <c r="G54" t="s">
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -6320,10 +6779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B828B6-BE11-4116-A181-72B4CE582051}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7993,6 +8452,9 @@
       <c r="B74" t="s">
         <v>663</v>
       </c>
+      <c r="C74">
+        <v>6.8</v>
+      </c>
       <c r="D74" t="s">
         <v>11</v>
       </c>
@@ -8000,10 +8462,135 @@
         <v>2024</v>
       </c>
       <c r="F74" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="G74" t="s">
         <v>231</v>
+      </c>
+      <c r="I74" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>45685</v>
+      </c>
+      <c r="B75" t="s">
+        <v>679</v>
+      </c>
+      <c r="C75">
+        <v>7.7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>51</v>
+      </c>
+      <c r="F75" t="s">
+        <v>49</v>
+      </c>
+      <c r="G75" t="s">
+        <v>442</v>
+      </c>
+      <c r="I75" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B76" s="16" t="str">
+        <f>"September 5"</f>
+        <v>September 5</v>
+      </c>
+      <c r="C76">
+        <v>7.8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76">
+        <v>2024</v>
+      </c>
+      <c r="F76" t="s">
+        <v>49</v>
+      </c>
+      <c r="G76" t="s">
+        <v>231</v>
+      </c>
+      <c r="I76" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>45687</v>
+      </c>
+      <c r="B77" t="s">
+        <v>684</v>
+      </c>
+      <c r="C77">
+        <v>7.2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77">
+        <v>2024</v>
+      </c>
+      <c r="F77" t="s">
+        <v>49</v>
+      </c>
+      <c r="G77" t="s">
+        <v>231</v>
+      </c>
+      <c r="I77" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>45691</v>
+      </c>
+      <c r="B78" t="s">
+        <v>709</v>
+      </c>
+      <c r="C78">
+        <v>7.4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78">
+        <v>2023</v>
+      </c>
+      <c r="F78" t="s">
+        <v>49</v>
+      </c>
+      <c r="G78" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>45692</v>
+      </c>
+      <c r="B79" t="s">
+        <v>708</v>
+      </c>
+      <c r="C79">
+        <v>7.6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" t="s">
+        <v>49</v>
+      </c>
+      <c r="G79" t="s">
+        <v>442</v>
+      </c>
+      <c r="I79" t="s">
+        <v>710</v>
       </c>
     </row>
   </sheetData>
@@ -8013,10 +8600,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1641D11-DBF0-4243-B307-B06B7AC69C48}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8561,6 +9148,48 @@
         <v>665</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>699</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B27" t="s">
+        <v>701</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>7.4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" t="s">
+        <v>441</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" t="s">
+        <v>716</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8568,10 +9197,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836806FA-EAD0-4C56-9A05-4DB9F5843EFD}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9180,6 +9809,58 @@
         <v>667</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45690</v>
+      </c>
+      <c r="B24" t="s">
+        <v>696</v>
+      </c>
+      <c r="C24">
+        <v>6.8</v>
+      </c>
+      <c r="D24">
+        <v>8.5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>697</v>
+      </c>
+      <c r="H24" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>45699</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25">
+        <v>7.4</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>718</v>
+      </c>
+      <c r="G25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" t="s">
+        <v>717</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9190,7 +9871,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9387,6 +10068,9 @@
       <c r="A11" t="s">
         <v>346</v>
       </c>
+      <c r="B11" s="2">
+        <v>45626</v>
+      </c>
       <c r="C11">
         <v>2024</v>
       </c>
@@ -9400,6 +10084,9 @@
         <v>8.4</v>
       </c>
       <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
         <v>49</v>
       </c>
       <c r="I11" t="s">
@@ -9426,7 +10113,7 @@
   <dimension ref="C5:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9604,6 +10291,9 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>45323</v>
+      </c>
       <c r="D14" t="s">
         <v>523</v>
       </c>
@@ -9615,6 +10305,12 @@
       </c>
       <c r="G14" t="s">
         <v>83</v>
+      </c>
+      <c r="H14">
+        <v>9.6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>702</v>
       </c>
     </row>
   </sheetData>
@@ -9821,7 +10517,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10089,7 +10785,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>